<commit_message>
Se incluye DarOpcionModulo y ValidarUrlIngreso
</commit_message>
<xml_diff>
--- a/Sevial/Sevial.DOC/Requerimientos/Tareas y historias.xlsx
+++ b/Sevial/Sevial.DOC/Requerimientos/Tareas y historias.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6585" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6585" firstSheet="9" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="TAREAS PROYECTO" sheetId="2" r:id="rId1"/>
@@ -2757,6 +2757,92 @@
         <a:xfrm>
           <a:off x="762000" y="5143500"/>
           <a:ext cx="6780952" cy="8800000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>675331</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>65881</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="4953000"/>
+          <a:ext cx="7552381" cy="6352381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>132474</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>56643</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="4000500"/>
+          <a:ext cx="7009524" cy="4057143"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5667,7 +5753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -6227,7 +6313,7 @@
   <dimension ref="B3:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6498,6 +6584,7 @@
     <hyperlink ref="C24" location="'HISTORIA 7'!A1" display="'HISTORIA 7'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6505,8 +6592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:C11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6704,6 +6791,7 @@
     <hyperlink ref="G4" location="SERVICIOS!A1" display="Lista Servicios"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11195,7 +11283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R110"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12002,7 +12090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R115"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -12945,7 +13033,7 @@
   <dimension ref="A1:R145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C10" sqref="C10:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se incluye servicio procesarArchivo
</commit_message>
<xml_diff>
--- a/Sevial/Sevial.DOC/Requerimientos/Tareas y historias.xlsx
+++ b/Sevial/Sevial.DOC/Requerimientos/Tareas y historias.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6585" firstSheet="4" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6585" firstSheet="6" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="TAREAS PROYECTO" sheetId="2" r:id="rId1"/>
@@ -1812,9 +1812,6 @@
     <t>Categoria: ESTADO_CARGUE</t>
   </si>
   <si>
-    <t>cargueInformacion/consultarArchivos</t>
-  </si>
-  <si>
     <t>Retorna la lista de archivos relacionados con el cargue de informacion y su estado</t>
   </si>
   <si>
@@ -1905,9 +1902,6 @@
     <t>Id del archivo a procesar</t>
   </si>
   <si>
-    <t>lista de archivos a procesar</t>
-  </si>
-  <si>
     <t>Regresar lista tarea iteracion</t>
   </si>
   <si>
@@ -2119,6 +2113,12 @@
   </si>
   <si>
     <t>parametro/DarListaCategoria</t>
+  </si>
+  <si>
+    <t>cargueInformacion/darArchivosCargue</t>
+  </si>
+  <si>
+    <t>lista de archivos a procesar (la lista viene el idTipoCarge,IdArchivo cada grupo seperado por ; )</t>
   </si>
 </sst>
 </file>
@@ -2924,6 +2924,92 @@
         <a:xfrm>
           <a:off x="762000" y="11811000"/>
           <a:ext cx="8409524" cy="6333333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>27617</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>8548</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="6096000"/>
+          <a:ext cx="7666667" cy="7819048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>389521</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>66048</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="4000500"/>
+          <a:ext cx="8028571" cy="5019048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5733,7 +5819,7 @@
         <v>29</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D77" s="1">
         <v>4</v>
@@ -5753,7 +5839,7 @@
         <v>29</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D78" s="1">
         <v>4</v>
@@ -5773,7 +5859,7 @@
         <v>65</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D79" s="1">
         <v>4</v>
@@ -6880,7 +6966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
@@ -6928,7 +7014,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -6999,10 +7085,10 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
@@ -7149,9 +7235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
+    <sheetView topLeftCell="A13" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7197,7 +7281,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>228</v>
+        <v>329</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -7216,7 +7300,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="40" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -7256,10 +7340,10 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="C12" s="23" t="s">
         <v>236</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>237</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -7268,10 +7352,10 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>238</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>239</v>
       </c>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
@@ -7328,10 +7412,10 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="C18" s="23" t="s">
         <v>230</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>231</v>
       </c>
       <c r="D18" s="23"/>
       <c r="E18" s="23"/>
@@ -7341,10 +7425,10 @@
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="25"/>
       <c r="C19" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="D19" s="23" t="s">
         <v>234</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>235</v>
       </c>
       <c r="E19" s="23"/>
       <c r="F19" s="23"/>
@@ -7353,10 +7437,10 @@
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="25"/>
       <c r="C20" s="23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E20" s="23"/>
       <c r="F20" s="23"/>
@@ -7365,10 +7449,10 @@
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="25"/>
       <c r="C21" s="23" t="s">
+        <v>239</v>
+      </c>
+      <c r="D21" s="23" t="s">
         <v>240</v>
-      </c>
-      <c r="D21" s="23" t="s">
-        <v>241</v>
       </c>
       <c r="E21" s="23"/>
       <c r="F21" s="23"/>
@@ -7377,10 +7461,10 @@
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="25"/>
       <c r="C22" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="D22" s="23" t="s">
         <v>242</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>243</v>
       </c>
       <c r="E22" s="23"/>
       <c r="F22" s="23"/>
@@ -7389,10 +7473,10 @@
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="25"/>
       <c r="C23" s="23" t="s">
+        <v>243</v>
+      </c>
+      <c r="D23" s="23" t="s">
         <v>244</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>245</v>
       </c>
       <c r="E23" s="23"/>
       <c r="F23" s="23"/>
@@ -7401,10 +7485,10 @@
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="25"/>
       <c r="C24" s="23" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E24" s="23"/>
       <c r="F24" s="23"/>
@@ -7413,10 +7497,10 @@
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="25"/>
       <c r="C25" s="23" t="s">
+        <v>246</v>
+      </c>
+      <c r="D25" s="23" t="s">
         <v>247</v>
-      </c>
-      <c r="D25" s="23" t="s">
-        <v>248</v>
       </c>
       <c r="E25" s="23"/>
       <c r="F25" s="23"/>
@@ -7425,10 +7509,10 @@
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="25"/>
       <c r="C26" s="23" t="s">
+        <v>248</v>
+      </c>
+      <c r="D26" s="23" t="s">
         <v>249</v>
-      </c>
-      <c r="D26" s="23" t="s">
-        <v>250</v>
       </c>
       <c r="E26" s="23"/>
       <c r="F26" s="23"/>
@@ -7437,10 +7521,10 @@
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="25"/>
       <c r="C27" s="23" t="s">
+        <v>250</v>
+      </c>
+      <c r="D27" s="23" t="s">
         <v>251</v>
-      </c>
-      <c r="D27" s="23" t="s">
-        <v>252</v>
       </c>
       <c r="E27" s="23"/>
       <c r="F27" s="23"/>
@@ -7449,10 +7533,10 @@
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="25"/>
       <c r="C28" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="D28" s="23" t="s">
         <v>253</v>
-      </c>
-      <c r="D28" s="23" t="s">
-        <v>254</v>
       </c>
       <c r="E28" s="23"/>
       <c r="F28" s="23"/>
@@ -7493,6 +7577,7 @@
     <hyperlink ref="C30" location="'HISTORIA 16'!A1" display="'HISTORIA 16'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7500,8 +7585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7548,7 +7633,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -7567,7 +7652,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="40" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -7607,10 +7692,10 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>259</v>
+        <v>330</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -7620,10 +7705,10 @@
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="48"/>
       <c r="C13" s="23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E13" s="23"/>
       <c r="F13" s="23"/>
@@ -7632,10 +7717,10 @@
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="48"/>
       <c r="C14" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E14" s="23"/>
       <c r="F14" s="23"/>
@@ -7724,6 +7809,7 @@
     <hyperlink ref="C20" location="'HISTORIA 16'!A1" display="'HISTORIA 16'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7779,7 +7865,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -7798,7 +7884,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="40" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -7838,10 +7924,10 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -7898,10 +7984,10 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
@@ -7911,10 +7997,10 @@
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="25"/>
       <c r="C18" s="23" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E18" s="23"/>
       <c r="F18" s="23"/>
@@ -7923,10 +8009,10 @@
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="25"/>
       <c r="C19" s="23" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E19" s="23"/>
       <c r="F19" s="23"/>
@@ -7935,10 +8021,10 @@
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="25"/>
       <c r="C20" s="23" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E20" s="23"/>
       <c r="F20" s="23"/>
@@ -7947,10 +8033,10 @@
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="25"/>
       <c r="C21" s="23" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E21" s="23"/>
       <c r="F21" s="23"/>
@@ -7959,10 +8045,10 @@
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="25"/>
       <c r="C22" s="23" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E22" s="23"/>
       <c r="F22" s="23"/>
@@ -7971,10 +8057,10 @@
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="25"/>
       <c r="C23" s="23" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E23" s="23"/>
       <c r="F23" s="23"/>
@@ -7983,10 +8069,10 @@
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="25"/>
       <c r="C24" s="23" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E24" s="23"/>
       <c r="F24" s="23"/>
@@ -7995,10 +8081,10 @@
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="25"/>
       <c r="C25" s="23" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E25" s="23"/>
       <c r="F25" s="23"/>
@@ -8007,10 +8093,10 @@
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="25"/>
       <c r="C26" s="23" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E26" s="23"/>
       <c r="F26" s="23"/>
@@ -8019,10 +8105,10 @@
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="25"/>
       <c r="C27" s="23" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E27" s="23"/>
       <c r="F27" s="23"/>
@@ -8031,10 +8117,10 @@
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="25"/>
       <c r="C28" s="23" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E28" s="23"/>
       <c r="F28" s="23"/>
@@ -8043,10 +8129,10 @@
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="25"/>
       <c r="C29" s="23" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E29" s="23"/>
       <c r="F29" s="23"/>
@@ -8055,10 +8141,10 @@
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="25"/>
       <c r="C30" s="23" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E30" s="23"/>
       <c r="F30" s="23"/>
@@ -8067,10 +8153,10 @@
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="25"/>
       <c r="C31" s="23" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E31" s="23"/>
       <c r="F31" s="23"/>
@@ -8079,10 +8165,10 @@
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="25"/>
       <c r="C32" s="23" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E32" s="23"/>
       <c r="F32" s="23"/>
@@ -8091,10 +8177,10 @@
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="25"/>
       <c r="C33" s="23" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E33" s="23"/>
       <c r="F33" s="23"/>
@@ -8103,10 +8189,10 @@
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="25"/>
       <c r="C34" s="23" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E34" s="23"/>
       <c r="F34" s="23"/>
@@ -8115,10 +8201,10 @@
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="25"/>
       <c r="C35" s="23" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E35" s="23"/>
       <c r="F35" s="23"/>
@@ -8127,10 +8213,10 @@
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="25"/>
       <c r="C36" s="23" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E36" s="23"/>
       <c r="F36" s="23"/>
@@ -8226,7 +8312,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -8245,7 +8331,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="40" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -8285,10 +8371,10 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -8433,7 +8519,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -8452,7 +8538,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="40" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -8492,10 +8578,10 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="23"/>
@@ -8504,10 +8590,10 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="23"/>
@@ -8516,10 +8602,10 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="23"/>
@@ -8528,10 +8614,10 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="23"/>
@@ -8540,10 +8626,10 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="25" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="23"/>
@@ -8552,10 +8638,10 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="23"/>
@@ -8564,10 +8650,10 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="25" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="23"/>
@@ -8576,10 +8662,10 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="25" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="23"/>
@@ -8588,10 +8674,10 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="25" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="23"/>
@@ -8600,10 +8686,10 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="25" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="23"/>
@@ -8612,10 +8698,10 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="25" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="23"/>
@@ -8624,10 +8710,10 @@
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="25" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="23"/>
@@ -8636,10 +8722,10 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="23"/>
@@ -8648,10 +8734,10 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="25" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="23"/>
@@ -8660,10 +8746,10 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="25" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="23"/>
@@ -8672,10 +8758,10 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="25" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="23"/>
@@ -8684,10 +8770,10 @@
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="25" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="23"/>
@@ -9403,7 +9489,7 @@
         <v>29</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D27" s="1">
         <v>4</v>
@@ -9426,7 +9512,7 @@
         <v>29</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D28" s="1">
         <v>4</v>
@@ -9546,7 +9632,7 @@
       <c r="F5" s="41"/>
       <c r="G5" s="41"/>
       <c r="H5" s="49" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I5" s="41"/>
     </row>
@@ -9669,7 +9755,7 @@
       </c>
       <c r="B13" t="str">
         <f>'SERVICIO 6'!C6</f>
-        <v>cargueInformacion/consultarArchivos</v>
+        <v>cargueInformacion/darArchivosCargue</v>
       </c>
       <c r="C13" s="46">
         <v>16</v>
@@ -9759,7 +9845,7 @@
         <v>Edicion Recaudo local - transferencias</v>
       </c>
       <c r="E18" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -9778,7 +9864,7 @@
         <v>Edicion Recaudo local - transferencias</v>
       </c>
       <c r="E19" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -9797,7 +9883,7 @@
         <v>Edicion Recaudo local - transferencias</v>
       </c>
       <c r="E20" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -9816,7 +9902,7 @@
         <v>Edicion Recaudo local - transferencias</v>
       </c>
       <c r="E21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -12178,7 +12264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R115"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
@@ -13012,7 +13098,7 @@
     </row>
     <row r="70" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C70" s="12">
         <v>6</v>
@@ -13273,7 +13359,7 @@
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="61" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C12" s="61"/>
       <c r="D12" s="61"/>
@@ -13327,7 +13413,7 @@
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="61" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C17" s="61"/>
       <c r="D17" s="61"/>
@@ -13383,7 +13469,7 @@
         <v>12</v>
       </c>
       <c r="C22" s="62" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D22" s="63"/>
       <c r="E22" s="63"/>
@@ -13395,7 +13481,7 @@
         <v>13</v>
       </c>
       <c r="C23" s="65" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D23" s="66"/>
       <c r="E23" s="66"/>
@@ -13407,7 +13493,7 @@
         <v>14</v>
       </c>
       <c r="C24" s="62" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D24" s="63"/>
       <c r="E24" s="63"/>
@@ -13427,7 +13513,7 @@
         <v>12</v>
       </c>
       <c r="C26" s="62" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D26" s="63"/>
       <c r="E26" s="63"/>
@@ -13439,7 +13525,7 @@
         <v>13</v>
       </c>
       <c r="C27" s="65" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D27" s="66"/>
       <c r="E27" s="66"/>
@@ -13451,7 +13537,7 @@
         <v>14</v>
       </c>
       <c r="C28" s="62" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D28" s="63"/>
       <c r="E28" s="63"/>
@@ -13471,7 +13557,7 @@
         <v>12</v>
       </c>
       <c r="C30" s="62" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D30" s="63"/>
       <c r="E30" s="63"/>
@@ -13483,7 +13569,7 @@
         <v>13</v>
       </c>
       <c r="C31" s="65" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D31" s="66"/>
       <c r="E31" s="66"/>
@@ -13495,7 +13581,7 @@
         <v>14</v>
       </c>
       <c r="C32" s="62" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D32" s="63"/>
       <c r="E32" s="63"/>
@@ -13505,7 +13591,7 @@
     <row r="33" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="19" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D33" s="20"/>
       <c r="E33" s="20"/>
@@ -13525,7 +13611,7 @@
         <v>12</v>
       </c>
       <c r="C35" s="62" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D35" s="63"/>
       <c r="E35" s="63"/>
@@ -13537,7 +13623,7 @@
         <v>13</v>
       </c>
       <c r="C36" s="65" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D36" s="66"/>
       <c r="E36" s="66"/>
@@ -13549,7 +13635,7 @@
         <v>14</v>
       </c>
       <c r="C37" s="62" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D37" s="63"/>
       <c r="E37" s="63"/>
@@ -13559,7 +13645,7 @@
     <row r="38" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="5"/>
       <c r="C38" s="19" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D38" s="20"/>
       <c r="E38" s="20"/>
@@ -13894,7 +13980,7 @@
     <row r="70" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="50"/>
       <c r="C70" s="73" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D70" s="73"/>
       <c r="E70" s="73"/>
@@ -14102,7 +14188,7 @@
       <c r="I88" s="51"/>
       <c r="J88" s="51"/>
       <c r="K88" s="7" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="89" spans="2:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -14227,7 +14313,7 @@
     </row>
     <row r="100" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B100" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C100" s="12">
         <v>8</v>

</xml_diff>

<commit_message>
Se incluye servicio DarTransferencias
</commit_message>
<xml_diff>
--- a/Sevial/Sevial.DOC/Requerimientos/Tareas y historias.xlsx
+++ b/Sevial/Sevial.DOC/Requerimientos/Tareas y historias.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6585" firstSheet="6" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6585" firstSheet="8" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="TAREAS PROYECTO" sheetId="2" r:id="rId1"/>
@@ -37,6 +37,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TAREAS PROYECTO'!$A$8:$G$76</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1126,7 +1127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="333">
   <si>
     <t>ID</t>
   </si>
@@ -1956,9 +1957,6 @@
     <t>Se muestra panel de edicion, se actualiza informacion, se procede a guardar</t>
   </si>
   <si>
-    <t>cargueInformacion/consultarTransferencias</t>
-  </si>
-  <si>
     <t>Consultar los registros de transferencias con un filtro dado</t>
   </si>
   <si>
@@ -2119,6 +2117,15 @@
   </si>
   <si>
     <t>lista de archivos a procesar (la lista viene el idTipoCarge,IdArchivo cada grupo seperado por ; )</t>
+  </si>
+  <si>
+    <t>bancoCuenta</t>
+  </si>
+  <si>
+    <t>Nombre banco - Numero Cuenta</t>
+  </si>
+  <si>
+    <t>informacion/darTransferencias</t>
   </si>
 </sst>
 </file>
@@ -3010,6 +3017,49 @@
         <a:xfrm>
           <a:off x="762000" y="4000500"/>
           <a:ext cx="8028571" cy="5019048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>427771</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>122798</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1238250" y="7143750"/>
+          <a:ext cx="6828571" cy="8219048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7014,7 +7064,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -7085,10 +7135,10 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
@@ -7281,7 +7331,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -7585,8 +7635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7695,7 +7745,7 @@
         <v>229</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -7815,10 +7865,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G38"/>
+  <dimension ref="B3:G36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7865,7 +7915,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>276</v>
+        <v>332</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -7884,7 +7934,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="40" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -7924,10 +7974,10 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
+        <v>277</v>
+      </c>
+      <c r="C12" s="23" t="s">
         <v>278</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>279</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -7984,10 +8034,10 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
+        <v>279</v>
+      </c>
+      <c r="C17" s="23" t="s">
         <v>280</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>281</v>
       </c>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
@@ -7997,10 +8047,10 @@
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="25"/>
       <c r="C18" s="23" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E18" s="23"/>
       <c r="F18" s="23"/>
@@ -8009,10 +8059,10 @@
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="25"/>
       <c r="C19" s="23" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E19" s="23"/>
       <c r="F19" s="23"/>
@@ -8021,10 +8071,10 @@
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="25"/>
       <c r="C20" s="23" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E20" s="23"/>
       <c r="F20" s="23"/>
@@ -8033,10 +8083,10 @@
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="25"/>
       <c r="C21" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E21" s="23"/>
       <c r="F21" s="23"/>
@@ -8045,10 +8095,10 @@
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="25"/>
       <c r="C22" s="23" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E22" s="23"/>
       <c r="F22" s="23"/>
@@ -8057,10 +8107,10 @@
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="25"/>
       <c r="C23" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E23" s="23"/>
       <c r="F23" s="23"/>
@@ -8069,10 +8119,10 @@
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="25"/>
       <c r="C24" s="23" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E24" s="23"/>
       <c r="F24" s="23"/>
@@ -8081,10 +8131,10 @@
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="25"/>
       <c r="C25" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E25" s="23"/>
       <c r="F25" s="23"/>
@@ -8093,10 +8143,10 @@
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="25"/>
       <c r="C26" s="23" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E26" s="23"/>
       <c r="F26" s="23"/>
@@ -8105,10 +8155,10 @@
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="25"/>
       <c r="C27" s="23" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E27" s="23"/>
       <c r="F27" s="23"/>
@@ -8117,10 +8167,10 @@
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="25"/>
       <c r="C28" s="23" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E28" s="23"/>
       <c r="F28" s="23"/>
@@ -8129,10 +8179,10 @@
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="25"/>
       <c r="C29" s="23" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E29" s="23"/>
       <c r="F29" s="23"/>
@@ -8141,10 +8191,10 @@
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="25"/>
       <c r="C30" s="23" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E30" s="23"/>
       <c r="F30" s="23"/>
@@ -8153,10 +8203,10 @@
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="25"/>
       <c r="C31" s="23" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E31" s="23"/>
       <c r="F31" s="23"/>
@@ -8165,10 +8215,10 @@
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="25"/>
       <c r="C32" s="23" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E32" s="23"/>
       <c r="F32" s="23"/>
@@ -8189,60 +8239,36 @@
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="25"/>
       <c r="C34" s="23" t="s">
-        <v>297</v>
+        <v>330</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>319</v>
+        <v>331</v>
       </c>
       <c r="E34" s="23"/>
       <c r="F34" s="23"/>
       <c r="G34" s="26"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="25"/>
-      <c r="C35" s="23" t="s">
-        <v>298</v>
-      </c>
-      <c r="D35" s="23" t="s">
-        <v>309</v>
-      </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="26"/>
+      <c r="B35" s="77" t="s">
+        <v>170</v>
+      </c>
+      <c r="C35" s="78"/>
+      <c r="D35" s="78"/>
+      <c r="E35" s="78"/>
+      <c r="F35" s="78"/>
+      <c r="G35" s="79"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="25"/>
-      <c r="C36" s="23" t="s">
-        <v>299</v>
-      </c>
-      <c r="D36" s="23" t="s">
-        <v>310</v>
-      </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="26"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="77" t="s">
-        <v>170</v>
-      </c>
-      <c r="C37" s="78"/>
-      <c r="D37" s="78"/>
-      <c r="E37" s="78"/>
-      <c r="F37" s="78"/>
-      <c r="G37" s="79"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="32" t="s">
+      <c r="B36" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="C38" s="47">
+      <c r="C36" s="47">
         <v>25</v>
       </c>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="34"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -8250,13 +8276,14 @@
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="B10:G10"/>
     <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B35:G35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G4" location="SERVICIOS!A1" display="Lista Servicios"/>
-    <hyperlink ref="C38" location="'HISTORIA 25'!A1" display="'HISTORIA 25'!A1"/>
+    <hyperlink ref="C36" location="'HISTORIA 25'!A1" display="'HISTORIA 25'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8312,7 +8339,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -8331,7 +8358,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="40" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -8371,10 +8398,10 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -8472,7 +8499,7 @@
   <dimension ref="B3:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8519,7 +8546,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -8538,7 +8565,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="40" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -8578,10 +8605,10 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="23"/>
@@ -8590,10 +8617,10 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="23"/>
@@ -8602,10 +8629,10 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="23"/>
@@ -8614,10 +8641,10 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="23"/>
@@ -8626,10 +8653,10 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="25" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="23"/>
@@ -8638,10 +8665,10 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="23"/>
@@ -8650,10 +8677,10 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="25" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="23"/>
@@ -8662,10 +8689,10 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="23"/>
@@ -8674,10 +8701,10 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="25" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="23"/>
@@ -8686,10 +8713,10 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="25" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="23"/>
@@ -8698,10 +8725,10 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="25" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="23"/>
@@ -8710,10 +8737,10 @@
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="23"/>
@@ -8722,10 +8749,10 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="23"/>
@@ -8734,10 +8761,10 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="25" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="23"/>
@@ -8746,10 +8773,10 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="25" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="23"/>
@@ -8758,10 +8785,10 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="25" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="23"/>
@@ -8770,10 +8797,10 @@
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="25" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="23"/>
@@ -9787,7 +9814,7 @@
       </c>
       <c r="B15" t="str">
         <f>'SERVICIO 8'!C6</f>
-        <v>cargueInformacion/consultarTransferencias</v>
+        <v>informacion/darTransferencias</v>
       </c>
       <c r="C15" s="36">
         <v>25</v>
@@ -9845,7 +9872,7 @@
         <v>Edicion Recaudo local - transferencias</v>
       </c>
       <c r="E18" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -9864,7 +9891,7 @@
         <v>Edicion Recaudo local - transferencias</v>
       </c>
       <c r="E19" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -9883,7 +9910,7 @@
         <v>Edicion Recaudo local - transferencias</v>
       </c>
       <c r="E20" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -9902,7 +9929,7 @@
         <v>Edicion Recaudo local - transferencias</v>
       </c>
       <c r="E21" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -13206,9 +13233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R145"/>
   <sheetViews>
-    <sheetView topLeftCell="C88" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
-    </sheetView>
+    <sheetView topLeftCell="A70" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13493,7 +13518,7 @@
         <v>14</v>
       </c>
       <c r="C24" s="62" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D24" s="63"/>
       <c r="E24" s="63"/>
@@ -14188,7 +14213,7 @@
       <c r="I88" s="51"/>
       <c r="J88" s="51"/>
       <c r="K88" s="7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="89" spans="2:11" s="7" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Traer opciones por módulo y usuario ok Plantilla 70% Seguridad por Url 60%
</commit_message>
<xml_diff>
--- a/Sevial/Sevial.DOC/Requerimientos/Tareas y historias.xlsx
+++ b/Sevial/Sevial.DOC/Requerimientos/Tareas y historias.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6585" firstSheet="8" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6585" firstSheet="6" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="TAREAS PROYECTO" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TAREAS PROYECTO'!$A$8:$G$76</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1127,7 +1126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="331">
   <si>
     <t>ID</t>
   </si>
@@ -1957,6 +1956,9 @@
     <t>Se muestra panel de edicion, se actualiza informacion, se procede a guardar</t>
   </si>
   <si>
+    <t>cargueInformacion/consultarTransferencias</t>
+  </si>
+  <si>
     <t>Consultar los registros de transferencias con un filtro dado</t>
   </si>
   <si>
@@ -2117,15 +2119,6 @@
   </si>
   <si>
     <t>lista de archivos a procesar (la lista viene el idTipoCarge,IdArchivo cada grupo seperado por ; )</t>
-  </si>
-  <si>
-    <t>bancoCuenta</t>
-  </si>
-  <si>
-    <t>Nombre banco - Numero Cuenta</t>
-  </si>
-  <si>
-    <t>informacion/darTransferencias</t>
   </si>
 </sst>
 </file>
@@ -3017,49 +3010,6 @@
         <a:xfrm>
           <a:off x="762000" y="4000500"/>
           <a:ext cx="8028571" cy="5019048"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>427771</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>122798</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1238250" y="7143750"/>
-          <a:ext cx="6828571" cy="8219048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7064,7 +7014,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -7135,10 +7085,10 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
@@ -7331,7 +7281,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -7635,8 +7585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G20"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7745,7 +7695,7 @@
         <v>229</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -7865,10 +7815,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G36"/>
+  <dimension ref="B3:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7915,7 +7865,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>332</v>
+        <v>276</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -7934,7 +7884,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="40" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -7974,10 +7924,10 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -8034,10 +7984,10 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
@@ -8047,10 +7997,10 @@
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="25"/>
       <c r="C18" s="23" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E18" s="23"/>
       <c r="F18" s="23"/>
@@ -8059,10 +8009,10 @@
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="25"/>
       <c r="C19" s="23" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E19" s="23"/>
       <c r="F19" s="23"/>
@@ -8071,10 +8021,10 @@
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="25"/>
       <c r="C20" s="23" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="E20" s="23"/>
       <c r="F20" s="23"/>
@@ -8083,10 +8033,10 @@
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="25"/>
       <c r="C21" s="23" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E21" s="23"/>
       <c r="F21" s="23"/>
@@ -8095,10 +8045,10 @@
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="25"/>
       <c r="C22" s="23" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E22" s="23"/>
       <c r="F22" s="23"/>
@@ -8107,10 +8057,10 @@
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="25"/>
       <c r="C23" s="23" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E23" s="23"/>
       <c r="F23" s="23"/>
@@ -8119,10 +8069,10 @@
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="25"/>
       <c r="C24" s="23" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E24" s="23"/>
       <c r="F24" s="23"/>
@@ -8131,10 +8081,10 @@
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="25"/>
       <c r="C25" s="23" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="E25" s="23"/>
       <c r="F25" s="23"/>
@@ -8143,10 +8093,10 @@
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="25"/>
       <c r="C26" s="23" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E26" s="23"/>
       <c r="F26" s="23"/>
@@ -8155,10 +8105,10 @@
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="25"/>
       <c r="C27" s="23" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E27" s="23"/>
       <c r="F27" s="23"/>
@@ -8167,10 +8117,10 @@
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="25"/>
       <c r="C28" s="23" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E28" s="23"/>
       <c r="F28" s="23"/>
@@ -8179,10 +8129,10 @@
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="25"/>
       <c r="C29" s="23" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E29" s="23"/>
       <c r="F29" s="23"/>
@@ -8191,10 +8141,10 @@
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="25"/>
       <c r="C30" s="23" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E30" s="23"/>
       <c r="F30" s="23"/>
@@ -8203,10 +8153,10 @@
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="25"/>
       <c r="C31" s="23" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E31" s="23"/>
       <c r="F31" s="23"/>
@@ -8215,10 +8165,10 @@
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="25"/>
       <c r="C32" s="23" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E32" s="23"/>
       <c r="F32" s="23"/>
@@ -8239,36 +8189,60 @@
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="25"/>
       <c r="C34" s="23" t="s">
-        <v>330</v>
+        <v>297</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="E34" s="23"/>
       <c r="F34" s="23"/>
       <c r="G34" s="26"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="77" t="s">
+      <c r="B35" s="25"/>
+      <c r="C35" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>309</v>
+      </c>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="26"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="25"/>
+      <c r="C36" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="26"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="77" t="s">
         <v>170</v>
       </c>
-      <c r="C35" s="78"/>
-      <c r="D35" s="78"/>
-      <c r="E35" s="78"/>
-      <c r="F35" s="78"/>
-      <c r="G35" s="79"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="32" t="s">
+      <c r="C37" s="78"/>
+      <c r="D37" s="78"/>
+      <c r="E37" s="78"/>
+      <c r="F37" s="78"/>
+      <c r="G37" s="79"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="C36" s="47">
+      <c r="C38" s="47">
         <v>25</v>
       </c>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="34"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -8276,14 +8250,13 @@
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="B10:G10"/>
     <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="B37:G37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G4" location="SERVICIOS!A1" display="Lista Servicios"/>
-    <hyperlink ref="C36" location="'HISTORIA 25'!A1" display="'HISTORIA 25'!A1"/>
+    <hyperlink ref="C38" location="'HISTORIA 25'!A1" display="'HISTORIA 25'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8339,7 +8312,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -8358,7 +8331,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="40" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -8398,10 +8371,10 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -8499,7 +8472,7 @@
   <dimension ref="B3:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8546,7 +8519,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -8565,7 +8538,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="40" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -8605,10 +8578,10 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="23"/>
@@ -8617,10 +8590,10 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="23"/>
@@ -8629,10 +8602,10 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="23"/>
@@ -8641,10 +8614,10 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="23"/>
@@ -8653,10 +8626,10 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="25" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="23"/>
@@ -8665,10 +8638,10 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="23"/>
@@ -8677,10 +8650,10 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="25" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="23"/>
@@ -8689,10 +8662,10 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="25" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="23"/>
@@ -8701,10 +8674,10 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="25" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="23"/>
@@ -8713,10 +8686,10 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="25" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="23"/>
@@ -8725,10 +8698,10 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="25" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="23"/>
@@ -8737,10 +8710,10 @@
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="25" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="23"/>
@@ -8749,10 +8722,10 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="23"/>
@@ -8761,10 +8734,10 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="25" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="23"/>
@@ -8773,10 +8746,10 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="25" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="23"/>
@@ -8785,10 +8758,10 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="25" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="23"/>
@@ -8797,10 +8770,10 @@
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="25" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="23"/>
@@ -9814,7 +9787,7 @@
       </c>
       <c r="B15" t="str">
         <f>'SERVICIO 8'!C6</f>
-        <v>informacion/darTransferencias</v>
+        <v>cargueInformacion/consultarTransferencias</v>
       </c>
       <c r="C15" s="36">
         <v>25</v>
@@ -9872,7 +9845,7 @@
         <v>Edicion Recaudo local - transferencias</v>
       </c>
       <c r="E18" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -9891,7 +9864,7 @@
         <v>Edicion Recaudo local - transferencias</v>
       </c>
       <c r="E19" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -9910,7 +9883,7 @@
         <v>Edicion Recaudo local - transferencias</v>
       </c>
       <c r="E20" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -9929,7 +9902,7 @@
         <v>Edicion Recaudo local - transferencias</v>
       </c>
       <c r="E21" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -13233,7 +13206,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R145"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView topLeftCell="C88" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13518,7 +13493,7 @@
         <v>14</v>
       </c>
       <c r="C24" s="62" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D24" s="63"/>
       <c r="E24" s="63"/>
@@ -14213,7 +14188,7 @@
       <c r="I88" s="51"/>
       <c r="J88" s="51"/>
       <c r="K88" s="7" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="89" spans="2:11" s="7" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Se crea servicio eliminarTransferencia
</commit_message>
<xml_diff>
--- a/Sevial/Sevial.DOC/Requerimientos/Tareas y historias.xlsx
+++ b/Sevial/Sevial.DOC/Requerimientos/Tareas y historias.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6585" firstSheet="6" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6585" firstSheet="8" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="TAREAS PROYECTO" sheetId="2" r:id="rId1"/>
@@ -1126,7 +1126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="332">
   <si>
     <t>ID</t>
   </si>
@@ -1956,9 +1956,6 @@
     <t>Se muestra panel de edicion, se actualiza informacion, se procede a guardar</t>
   </si>
   <si>
-    <t>cargueInformacion/consultarTransferencias</t>
-  </si>
-  <si>
     <t>Consultar los registros de transferencias con un filtro dado</t>
   </si>
   <si>
@@ -2037,9 +2034,6 @@
     <t xml:space="preserve">Solo se muestran los 50 primeros registros </t>
   </si>
   <si>
-    <t>cargueInformacion/eliminarTransferencia</t>
-  </si>
-  <si>
     <t>elimina la informacion de una transferencia registrada</t>
   </si>
   <si>
@@ -2119,6 +2113,15 @@
   </si>
   <si>
     <t>lista de archivos a procesar (la lista viene el idTipoCarge,IdArchivo cada grupo seperado por ; )</t>
+  </si>
+  <si>
+    <t>informacion/darTransferencias</t>
+  </si>
+  <si>
+    <t>informacion/eliminarTransferencia</t>
+  </si>
+  <si>
+    <t>idRegistro</t>
   </si>
 </sst>
 </file>
@@ -2518,16 +2521,19 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2540,14 +2546,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3010,6 +3013,92 @@
         <a:xfrm>
           <a:off x="762000" y="4000500"/>
           <a:ext cx="8028571" cy="5019048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>46759</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>8524</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="7620000"/>
+          <a:ext cx="6923809" cy="8009524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>351521</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>104143</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="4000500"/>
+          <a:ext cx="7228571" cy="5057143"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7014,7 +7103,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -7085,10 +7174,10 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
@@ -7281,7 +7370,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -7585,7 +7674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -7695,7 +7784,7 @@
         <v>229</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -7817,8 +7906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7865,7 +7954,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>276</v>
+        <v>329</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -7884,7 +7973,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="40" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -7924,10 +8013,10 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
+        <v>277</v>
+      </c>
+      <c r="C12" s="23" t="s">
         <v>278</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>279</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -7984,10 +8073,10 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
+        <v>279</v>
+      </c>
+      <c r="C17" s="23" t="s">
         <v>280</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>281</v>
       </c>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
@@ -7997,10 +8086,10 @@
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="25"/>
       <c r="C18" s="23" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E18" s="23"/>
       <c r="F18" s="23"/>
@@ -8009,10 +8098,10 @@
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="25"/>
       <c r="C19" s="23" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E19" s="23"/>
       <c r="F19" s="23"/>
@@ -8021,10 +8110,10 @@
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="25"/>
       <c r="C20" s="23" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E20" s="23"/>
       <c r="F20" s="23"/>
@@ -8033,10 +8122,10 @@
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="25"/>
       <c r="C21" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E21" s="23"/>
       <c r="F21" s="23"/>
@@ -8045,10 +8134,10 @@
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="25"/>
       <c r="C22" s="23" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E22" s="23"/>
       <c r="F22" s="23"/>
@@ -8057,10 +8146,10 @@
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="25"/>
       <c r="C23" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E23" s="23"/>
       <c r="F23" s="23"/>
@@ -8069,10 +8158,10 @@
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="25"/>
       <c r="C24" s="23" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E24" s="23"/>
       <c r="F24" s="23"/>
@@ -8081,10 +8170,10 @@
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="25"/>
       <c r="C25" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E25" s="23"/>
       <c r="F25" s="23"/>
@@ -8093,10 +8182,10 @@
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="25"/>
       <c r="C26" s="23" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E26" s="23"/>
       <c r="F26" s="23"/>
@@ -8105,10 +8194,10 @@
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="25"/>
       <c r="C27" s="23" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E27" s="23"/>
       <c r="F27" s="23"/>
@@ -8117,10 +8206,10 @@
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="25"/>
       <c r="C28" s="23" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E28" s="23"/>
       <c r="F28" s="23"/>
@@ -8129,10 +8218,10 @@
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="25"/>
       <c r="C29" s="23" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E29" s="23"/>
       <c r="F29" s="23"/>
@@ -8141,10 +8230,10 @@
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="25"/>
       <c r="C30" s="23" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E30" s="23"/>
       <c r="F30" s="23"/>
@@ -8153,10 +8242,10 @@
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="25"/>
       <c r="C31" s="23" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E31" s="23"/>
       <c r="F31" s="23"/>
@@ -8165,10 +8254,10 @@
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="25"/>
       <c r="C32" s="23" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E32" s="23"/>
       <c r="F32" s="23"/>
@@ -8177,10 +8266,10 @@
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="25"/>
       <c r="C33" s="23" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E33" s="23"/>
       <c r="F33" s="23"/>
@@ -8189,10 +8278,10 @@
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="25"/>
       <c r="C34" s="23" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E34" s="23"/>
       <c r="F34" s="23"/>
@@ -8201,10 +8290,10 @@
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="25"/>
       <c r="C35" s="23" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E35" s="23"/>
       <c r="F35" s="23"/>
@@ -8213,10 +8302,10 @@
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="25"/>
       <c r="C36" s="23" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E36" s="23"/>
       <c r="F36" s="23"/>
@@ -8257,6 +8346,7 @@
     <hyperlink ref="C38" location="'HISTORIA 25'!A1" display="'HISTORIA 25'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8264,8 +8354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8312,7 +8402,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>303</v>
+        <v>330</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -8331,7 +8421,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="40" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -8371,10 +8461,10 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>300</v>
+        <v>331</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -8464,6 +8554,7 @@
     <hyperlink ref="C18" location="'HISTORIA 25'!A1" display="'HISTORIA 25'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8519,7 +8610,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -8538,7 +8629,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="40" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -8578,10 +8669,10 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="23"/>
@@ -8590,10 +8681,10 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="23"/>
@@ -8602,10 +8693,10 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="23"/>
@@ -8614,10 +8705,10 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="23"/>
@@ -8626,10 +8717,10 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="25" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="23"/>
@@ -8638,10 +8729,10 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="23"/>
@@ -8650,10 +8741,10 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="25" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="23"/>
@@ -8662,10 +8753,10 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="23"/>
@@ -8674,10 +8765,10 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="25" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="23"/>
@@ -8686,10 +8777,10 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="25" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="23"/>
@@ -8698,10 +8789,10 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="25" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="23"/>
@@ -8710,10 +8801,10 @@
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="23"/>
@@ -8722,10 +8813,10 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="23"/>
@@ -8734,10 +8825,10 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="25" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="23"/>
@@ -8746,10 +8837,10 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="25" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="23"/>
@@ -8758,10 +8849,10 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="25" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="23"/>
@@ -8770,10 +8861,10 @@
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="25" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="23"/>
@@ -9787,7 +9878,7 @@
       </c>
       <c r="B15" t="str">
         <f>'SERVICIO 8'!C6</f>
-        <v>cargueInformacion/consultarTransferencias</v>
+        <v>informacion/darTransferencias</v>
       </c>
       <c r="C15" s="36">
         <v>25</v>
@@ -9803,7 +9894,7 @@
       </c>
       <c r="B16" t="str">
         <f>'SERVICIO 9'!C6</f>
-        <v>cargueInformacion/eliminarTransferencia</v>
+        <v>informacion/eliminarTransferencia</v>
       </c>
       <c r="C16" s="36">
         <v>25</v>
@@ -9845,7 +9936,7 @@
         <v>Edicion Recaudo local - transferencias</v>
       </c>
       <c r="E18" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -9864,7 +9955,7 @@
         <v>Edicion Recaudo local - transferencias</v>
       </c>
       <c r="E19" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -9883,7 +9974,7 @@
         <v>Edicion Recaudo local - transferencias</v>
       </c>
       <c r="E20" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -9902,7 +9993,7 @@
         <v>Edicion Recaudo local - transferencias</v>
       </c>
       <c r="E21" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -9995,11 +10086,11 @@
     <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -10037,14 +10128,14 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
@@ -10074,14 +10165,14 @@
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="59" t="str">
+      <c r="C9" s="70" t="str">
         <f>'TAREAS PROYECTO'!B9</f>
         <v>Seguridad</v>
       </c>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -10089,134 +10180,134 @@
       <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="58" t="str">
+      <c r="C10" s="69" t="str">
         <f>'TAREAS PROYECTO'!C9</f>
         <v>Inicio de sesion</v>
       </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="61" t="s">
+      <c r="B12" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
       <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="59" t="s">
         <v>101</v>
       </c>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
-      <c r="B18" s="61"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="61"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="61"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59"/>
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
-      <c r="B19" s="61"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="61"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59"/>
       <c r="H19" s="7"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
-      <c r="B20" s="61"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="61"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59"/>
       <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
-      <c r="B21" s="60" t="s">
+      <c r="B21" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="60"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="60"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="62"/>
       <c r="H21" s="7"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -10224,13 +10315,13 @@
       <c r="B22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="62" t="s">
+      <c r="C22" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="65"/>
       <c r="H22" s="7"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -10238,13 +10329,13 @@
       <c r="B23" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="65" t="s">
+      <c r="C23" s="66" t="s">
         <v>103</v>
       </c>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="68"/>
       <c r="H23" s="7"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -10252,13 +10343,13 @@
       <c r="B24" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="62" t="s">
+      <c r="C24" s="63" t="s">
         <v>104</v>
       </c>
-      <c r="D24" s="63"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="63"/>
-      <c r="G24" s="64"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="65"/>
       <c r="H24" s="7"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -10276,13 +10367,13 @@
       <c r="B26" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="62" t="s">
+      <c r="C26" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="D26" s="63"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="63"/>
-      <c r="G26" s="64"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="64"/>
+      <c r="G26" s="65"/>
       <c r="H26" s="7"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -10290,13 +10381,13 @@
       <c r="B27" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="65" t="s">
+      <c r="C27" s="66" t="s">
         <v>105</v>
       </c>
-      <c r="D27" s="66"/>
-      <c r="E27" s="66"/>
-      <c r="F27" s="66"/>
-      <c r="G27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="68"/>
       <c r="H27" s="7"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -10304,13 +10395,13 @@
       <c r="B28" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="62" t="s">
+      <c r="C28" s="63" t="s">
         <v>109</v>
       </c>
-      <c r="D28" s="63"/>
-      <c r="E28" s="63"/>
-      <c r="F28" s="63"/>
-      <c r="G28" s="64"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="64"/>
+      <c r="F28" s="64"/>
+      <c r="G28" s="65"/>
       <c r="H28" s="7"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -10328,13 +10419,13 @@
       <c r="B30" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="62" t="s">
+      <c r="C30" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="D30" s="63"/>
-      <c r="E30" s="63"/>
-      <c r="F30" s="63"/>
-      <c r="G30" s="64"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="64"/>
+      <c r="G30" s="65"/>
       <c r="H30" s="7"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -10342,13 +10433,13 @@
       <c r="B31" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="65" t="s">
+      <c r="C31" s="66" t="s">
         <v>107</v>
       </c>
-      <c r="D31" s="66"/>
-      <c r="E31" s="66"/>
-      <c r="F31" s="66"/>
-      <c r="G31" s="67"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="68"/>
       <c r="H31" s="7"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -10356,13 +10447,13 @@
       <c r="B32" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="62" t="s">
+      <c r="C32" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="D32" s="63"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="63"/>
-      <c r="G32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="64"/>
+      <c r="G32" s="65"/>
       <c r="H32" s="7"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -10377,174 +10468,174 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
-      <c r="B34" s="60" t="s">
+      <c r="B34" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="C34" s="60"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="60"/>
-      <c r="F34" s="60"/>
-      <c r="G34" s="60"/>
+      <c r="C34" s="62"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="62"/>
+      <c r="F34" s="62"/>
+      <c r="G34" s="62"/>
       <c r="H34" s="7"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
-      <c r="B35" s="70"/>
-      <c r="C35" s="70"/>
-      <c r="D35" s="70"/>
-      <c r="E35" s="70"/>
-      <c r="F35" s="70"/>
-      <c r="G35" s="70"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="61"/>
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
-      <c r="B36" s="70"/>
-      <c r="C36" s="70"/>
-      <c r="D36" s="70"/>
-      <c r="E36" s="70"/>
-      <c r="F36" s="70"/>
-      <c r="G36" s="70"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="61"/>
+      <c r="F36" s="61"/>
+      <c r="G36" s="61"/>
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
-      <c r="B37" s="70"/>
-      <c r="C37" s="70"/>
-      <c r="D37" s="70"/>
-      <c r="E37" s="70"/>
-      <c r="F37" s="70"/>
-      <c r="G37" s="70"/>
+      <c r="B37" s="61"/>
+      <c r="C37" s="61"/>
+      <c r="D37" s="61"/>
+      <c r="E37" s="61"/>
+      <c r="F37" s="61"/>
+      <c r="G37" s="61"/>
       <c r="H37" s="7"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
-      <c r="B38" s="70"/>
-      <c r="C38" s="70"/>
-      <c r="D38" s="70"/>
-      <c r="E38" s="70"/>
-      <c r="F38" s="70"/>
-      <c r="G38" s="70"/>
+      <c r="B38" s="61"/>
+      <c r="C38" s="61"/>
+      <c r="D38" s="61"/>
+      <c r="E38" s="61"/>
+      <c r="F38" s="61"/>
+      <c r="G38" s="61"/>
       <c r="H38" s="7"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="70"/>
-      <c r="C39" s="70"/>
-      <c r="D39" s="70"/>
-      <c r="E39" s="70"/>
-      <c r="F39" s="70"/>
-      <c r="G39" s="70"/>
+      <c r="B39" s="61"/>
+      <c r="C39" s="61"/>
+      <c r="D39" s="61"/>
+      <c r="E39" s="61"/>
+      <c r="F39" s="61"/>
+      <c r="G39" s="61"/>
       <c r="H39" s="7"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
-      <c r="B40" s="70"/>
-      <c r="C40" s="70"/>
-      <c r="D40" s="70"/>
-      <c r="E40" s="70"/>
-      <c r="F40" s="70"/>
-      <c r="G40" s="70"/>
+      <c r="B40" s="61"/>
+      <c r="C40" s="61"/>
+      <c r="D40" s="61"/>
+      <c r="E40" s="61"/>
+      <c r="F40" s="61"/>
+      <c r="G40" s="61"/>
       <c r="H40" s="7"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
-      <c r="B41" s="70"/>
-      <c r="C41" s="70"/>
-      <c r="D41" s="70"/>
-      <c r="E41" s="70"/>
-      <c r="F41" s="70"/>
-      <c r="G41" s="70"/>
+      <c r="B41" s="61"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="61"/>
+      <c r="E41" s="61"/>
+      <c r="F41" s="61"/>
+      <c r="G41" s="61"/>
       <c r="H41" s="7"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
-      <c r="B42" s="70"/>
-      <c r="C42" s="70"/>
-      <c r="D42" s="70"/>
-      <c r="E42" s="70"/>
-      <c r="F42" s="70"/>
-      <c r="G42" s="70"/>
+      <c r="B42" s="61"/>
+      <c r="C42" s="61"/>
+      <c r="D42" s="61"/>
+      <c r="E42" s="61"/>
+      <c r="F42" s="61"/>
+      <c r="G42" s="61"/>
       <c r="H42" s="7"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
-      <c r="B43" s="70"/>
-      <c r="C43" s="70"/>
-      <c r="D43" s="70"/>
-      <c r="E43" s="70"/>
-      <c r="F43" s="70"/>
-      <c r="G43" s="70"/>
+      <c r="B43" s="61"/>
+      <c r="C43" s="61"/>
+      <c r="D43" s="61"/>
+      <c r="E43" s="61"/>
+      <c r="F43" s="61"/>
+      <c r="G43" s="61"/>
       <c r="H43" s="7"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
-      <c r="B44" s="70"/>
-      <c r="C44" s="70"/>
-      <c r="D44" s="70"/>
-      <c r="E44" s="70"/>
-      <c r="F44" s="70"/>
-      <c r="G44" s="70"/>
+      <c r="B44" s="61"/>
+      <c r="C44" s="61"/>
+      <c r="D44" s="61"/>
+      <c r="E44" s="61"/>
+      <c r="F44" s="61"/>
+      <c r="G44" s="61"/>
       <c r="H44" s="7"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
-      <c r="B45" s="70"/>
-      <c r="C45" s="70"/>
-      <c r="D45" s="70"/>
-      <c r="E45" s="70"/>
-      <c r="F45" s="70"/>
-      <c r="G45" s="70"/>
+      <c r="B45" s="61"/>
+      <c r="C45" s="61"/>
+      <c r="D45" s="61"/>
+      <c r="E45" s="61"/>
+      <c r="F45" s="61"/>
+      <c r="G45" s="61"/>
       <c r="H45" s="7"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
-      <c r="B46" s="70"/>
-      <c r="C46" s="70"/>
-      <c r="D46" s="70"/>
-      <c r="E46" s="70"/>
-      <c r="F46" s="70"/>
-      <c r="G46" s="70"/>
+      <c r="B46" s="61"/>
+      <c r="C46" s="61"/>
+      <c r="D46" s="61"/>
+      <c r="E46" s="61"/>
+      <c r="F46" s="61"/>
+      <c r="G46" s="61"/>
       <c r="H46" s="7"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
-      <c r="B47" s="70"/>
-      <c r="C47" s="70"/>
-      <c r="D47" s="70"/>
-      <c r="E47" s="70"/>
-      <c r="F47" s="70"/>
-      <c r="G47" s="70"/>
+      <c r="B47" s="61"/>
+      <c r="C47" s="61"/>
+      <c r="D47" s="61"/>
+      <c r="E47" s="61"/>
+      <c r="F47" s="61"/>
+      <c r="G47" s="61"/>
       <c r="H47" s="7"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
-      <c r="B48" s="70"/>
-      <c r="C48" s="70"/>
-      <c r="D48" s="70"/>
-      <c r="E48" s="70"/>
-      <c r="F48" s="70"/>
-      <c r="G48" s="70"/>
+      <c r="B48" s="61"/>
+      <c r="C48" s="61"/>
+      <c r="D48" s="61"/>
+      <c r="E48" s="61"/>
+      <c r="F48" s="61"/>
+      <c r="G48" s="61"/>
       <c r="H48" s="7"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
-      <c r="B49" s="70"/>
-      <c r="C49" s="70"/>
-      <c r="D49" s="70"/>
-      <c r="E49" s="70"/>
-      <c r="F49" s="70"/>
-      <c r="G49" s="70"/>
+      <c r="B49" s="61"/>
+      <c r="C49" s="61"/>
+      <c r="D49" s="61"/>
+      <c r="E49" s="61"/>
+      <c r="F49" s="61"/>
+      <c r="G49" s="61"/>
       <c r="H49" s="7"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
-      <c r="B50" s="70"/>
-      <c r="C50" s="70"/>
-      <c r="D50" s="70"/>
-      <c r="E50" s="70"/>
-      <c r="F50" s="70"/>
-      <c r="G50" s="70"/>
+      <c r="B50" s="61"/>
+      <c r="C50" s="61"/>
+      <c r="D50" s="61"/>
+      <c r="E50" s="61"/>
+      <c r="F50" s="61"/>
+      <c r="G50" s="61"/>
       <c r="H50" s="7"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -10606,6 +10697,16 @@
     <row r="96" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="B19:G19"/>
     <mergeCell ref="B20:G20"/>
@@ -10622,16 +10723,6 @@
     <mergeCell ref="B21:G21"/>
     <mergeCell ref="B17:G17"/>
     <mergeCell ref="B18:G18"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
   </mergeCells>
   <conditionalFormatting sqref="G8">
     <cfRule type="iconSet" priority="1">
@@ -10692,11 +10783,11 @@
     <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -10734,14 +10825,14 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
@@ -10771,14 +10862,14 @@
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="59" t="str">
+      <c r="C9" s="70" t="str">
         <f>'TAREAS PROYECTO'!B14</f>
         <v>Seguridad</v>
       </c>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -10786,220 +10877,220 @@
       <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="58" t="str">
+      <c r="C10" s="69" t="str">
         <f>'TAREAS PROYECTO'!C14</f>
         <v>Modulos asignados</v>
       </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="61" t="s">
+      <c r="B12" s="59" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
       <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="59" t="s">
         <v>114</v>
       </c>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
-      <c r="B18" s="61"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="61"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="61"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59"/>
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="60"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
       <c r="H19" s="7"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
-      <c r="B20" s="62" t="s">
+      <c r="B20" s="63" t="s">
         <v>116</v>
       </c>
-      <c r="C20" s="63"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
-      <c r="G20" s="64"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="65"/>
       <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
-      <c r="B21" s="62" t="s">
+      <c r="B21" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63"/>
-      <c r="G21" s="64"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="65"/>
       <c r="H21" s="7"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
-      <c r="B22" s="62" t="s">
+      <c r="B22" s="63" t="s">
         <v>117</v>
       </c>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="64"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="65"/>
       <c r="H22" s="7"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
-      <c r="B23" s="62" t="s">
+      <c r="B23" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63"/>
-      <c r="G23" s="64"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="65"/>
       <c r="H23" s="7"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
-      <c r="B24" s="62" t="s">
+      <c r="B24" s="63" t="s">
         <v>118</v>
       </c>
-      <c r="C24" s="63"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="63"/>
-      <c r="G24" s="64"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="65"/>
       <c r="H24" s="7"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
-      <c r="B25" s="61" t="s">
+      <c r="B25" s="59" t="s">
         <v>119</v>
       </c>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="61"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
       <c r="H25" s="7"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
-      <c r="B26" s="62" t="s">
+      <c r="B26" s="63" t="s">
         <v>120</v>
       </c>
-      <c r="C26" s="63"/>
-      <c r="D26" s="63"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="63"/>
-      <c r="G26" s="64"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="64"/>
+      <c r="G26" s="65"/>
       <c r="H26" s="7"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
-      <c r="B27" s="62"/>
-      <c r="C27" s="63"/>
-      <c r="D27" s="63"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="64"/>
+      <c r="B27" s="63"/>
+      <c r="C27" s="64"/>
+      <c r="D27" s="64"/>
+      <c r="E27" s="64"/>
+      <c r="F27" s="64"/>
+      <c r="G27" s="65"/>
       <c r="H27" s="7"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
-      <c r="B28" s="60" t="s">
+      <c r="B28" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="60"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="60"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="62"/>
       <c r="H28" s="7"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -11007,13 +11098,13 @@
       <c r="B29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="62" t="s">
+      <c r="C29" s="63" t="s">
         <v>115</v>
       </c>
-      <c r="D29" s="63"/>
-      <c r="E29" s="63"/>
-      <c r="F29" s="63"/>
-      <c r="G29" s="64"/>
+      <c r="D29" s="64"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="64"/>
+      <c r="G29" s="65"/>
       <c r="H29" s="7"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -11021,13 +11112,13 @@
       <c r="B30" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="65" t="s">
+      <c r="C30" s="66" t="s">
         <v>103</v>
       </c>
-      <c r="D30" s="66"/>
-      <c r="E30" s="66"/>
-      <c r="F30" s="66"/>
-      <c r="G30" s="67"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="68"/>
       <c r="H30" s="7"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -11035,13 +11126,13 @@
       <c r="B31" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="62" t="s">
+      <c r="C31" s="63" t="s">
         <v>104</v>
       </c>
-      <c r="D31" s="63"/>
-      <c r="E31" s="63"/>
-      <c r="F31" s="63"/>
-      <c r="G31" s="64"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="65"/>
       <c r="H31" s="7"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -11066,284 +11157,284 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
-      <c r="B34" s="60" t="s">
+      <c r="B34" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="C34" s="60"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="60"/>
-      <c r="F34" s="60"/>
-      <c r="G34" s="60"/>
+      <c r="C34" s="62"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="62"/>
+      <c r="F34" s="62"/>
+      <c r="G34" s="62"/>
       <c r="H34" s="7"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
-      <c r="B35" s="70"/>
-      <c r="C35" s="70"/>
-      <c r="D35" s="70"/>
-      <c r="E35" s="70"/>
-      <c r="F35" s="70"/>
-      <c r="G35" s="70"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="61"/>
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
-      <c r="B36" s="70"/>
-      <c r="C36" s="70"/>
-      <c r="D36" s="70"/>
-      <c r="E36" s="70"/>
-      <c r="F36" s="70"/>
-      <c r="G36" s="70"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="61"/>
+      <c r="F36" s="61"/>
+      <c r="G36" s="61"/>
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
-      <c r="B37" s="70"/>
-      <c r="C37" s="70"/>
-      <c r="D37" s="70"/>
-      <c r="E37" s="70"/>
-      <c r="F37" s="70"/>
-      <c r="G37" s="70"/>
+      <c r="B37" s="61"/>
+      <c r="C37" s="61"/>
+      <c r="D37" s="61"/>
+      <c r="E37" s="61"/>
+      <c r="F37" s="61"/>
+      <c r="G37" s="61"/>
       <c r="H37" s="7"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
-      <c r="B38" s="70"/>
-      <c r="C38" s="70"/>
-      <c r="D38" s="70"/>
-      <c r="E38" s="70"/>
-      <c r="F38" s="70"/>
-      <c r="G38" s="70"/>
+      <c r="B38" s="61"/>
+      <c r="C38" s="61"/>
+      <c r="D38" s="61"/>
+      <c r="E38" s="61"/>
+      <c r="F38" s="61"/>
+      <c r="G38" s="61"/>
       <c r="H38" s="7"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="70"/>
-      <c r="C39" s="70"/>
-      <c r="D39" s="70"/>
-      <c r="E39" s="70"/>
-      <c r="F39" s="70"/>
-      <c r="G39" s="70"/>
+      <c r="B39" s="61"/>
+      <c r="C39" s="61"/>
+      <c r="D39" s="61"/>
+      <c r="E39" s="61"/>
+      <c r="F39" s="61"/>
+      <c r="G39" s="61"/>
       <c r="H39" s="7"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
-      <c r="B40" s="70"/>
-      <c r="C40" s="70"/>
-      <c r="D40" s="70"/>
-      <c r="E40" s="70"/>
-      <c r="F40" s="70"/>
-      <c r="G40" s="70"/>
+      <c r="B40" s="61"/>
+      <c r="C40" s="61"/>
+      <c r="D40" s="61"/>
+      <c r="E40" s="61"/>
+      <c r="F40" s="61"/>
+      <c r="G40" s="61"/>
       <c r="H40" s="7"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
-      <c r="B41" s="70"/>
-      <c r="C41" s="70"/>
-      <c r="D41" s="70"/>
-      <c r="E41" s="70"/>
-      <c r="F41" s="70"/>
-      <c r="G41" s="70"/>
+      <c r="B41" s="61"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="61"/>
+      <c r="E41" s="61"/>
+      <c r="F41" s="61"/>
+      <c r="G41" s="61"/>
       <c r="H41" s="7"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
-      <c r="B42" s="70"/>
-      <c r="C42" s="70"/>
-      <c r="D42" s="70"/>
-      <c r="E42" s="70"/>
-      <c r="F42" s="70"/>
-      <c r="G42" s="70"/>
+      <c r="B42" s="61"/>
+      <c r="C42" s="61"/>
+      <c r="D42" s="61"/>
+      <c r="E42" s="61"/>
+      <c r="F42" s="61"/>
+      <c r="G42" s="61"/>
       <c r="H42" s="7"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
-      <c r="B43" s="70"/>
-      <c r="C43" s="70"/>
-      <c r="D43" s="70"/>
-      <c r="E43" s="70"/>
-      <c r="F43" s="70"/>
-      <c r="G43" s="70"/>
+      <c r="B43" s="61"/>
+      <c r="C43" s="61"/>
+      <c r="D43" s="61"/>
+      <c r="E43" s="61"/>
+      <c r="F43" s="61"/>
+      <c r="G43" s="61"/>
       <c r="H43" s="7"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
-      <c r="B44" s="70"/>
-      <c r="C44" s="70"/>
-      <c r="D44" s="70"/>
-      <c r="E44" s="70"/>
-      <c r="F44" s="70"/>
-      <c r="G44" s="70"/>
+      <c r="B44" s="61"/>
+      <c r="C44" s="61"/>
+      <c r="D44" s="61"/>
+      <c r="E44" s="61"/>
+      <c r="F44" s="61"/>
+      <c r="G44" s="61"/>
       <c r="H44" s="7"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
-      <c r="B45" s="70"/>
-      <c r="C45" s="70"/>
-      <c r="D45" s="70"/>
-      <c r="E45" s="70"/>
-      <c r="F45" s="70"/>
-      <c r="G45" s="70"/>
+      <c r="B45" s="61"/>
+      <c r="C45" s="61"/>
+      <c r="D45" s="61"/>
+      <c r="E45" s="61"/>
+      <c r="F45" s="61"/>
+      <c r="G45" s="61"/>
       <c r="H45" s="7"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
-      <c r="B46" s="70"/>
-      <c r="C46" s="70"/>
-      <c r="D46" s="70"/>
-      <c r="E46" s="70"/>
-      <c r="F46" s="70"/>
-      <c r="G46" s="70"/>
+      <c r="B46" s="61"/>
+      <c r="C46" s="61"/>
+      <c r="D46" s="61"/>
+      <c r="E46" s="61"/>
+      <c r="F46" s="61"/>
+      <c r="G46" s="61"/>
       <c r="H46" s="7"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
-      <c r="B47" s="70"/>
-      <c r="C47" s="70"/>
-      <c r="D47" s="70"/>
-      <c r="E47" s="70"/>
-      <c r="F47" s="70"/>
-      <c r="G47" s="70"/>
+      <c r="B47" s="61"/>
+      <c r="C47" s="61"/>
+      <c r="D47" s="61"/>
+      <c r="E47" s="61"/>
+      <c r="F47" s="61"/>
+      <c r="G47" s="61"/>
       <c r="H47" s="7"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
-      <c r="B48" s="70"/>
-      <c r="C48" s="70"/>
-      <c r="D48" s="70"/>
-      <c r="E48" s="70"/>
-      <c r="F48" s="70"/>
-      <c r="G48" s="70"/>
+      <c r="B48" s="61"/>
+      <c r="C48" s="61"/>
+      <c r="D48" s="61"/>
+      <c r="E48" s="61"/>
+      <c r="F48" s="61"/>
+      <c r="G48" s="61"/>
       <c r="H48" s="7"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
-      <c r="B49" s="70"/>
-      <c r="C49" s="70"/>
-      <c r="D49" s="70"/>
-      <c r="E49" s="70"/>
-      <c r="F49" s="70"/>
-      <c r="G49" s="70"/>
+      <c r="B49" s="61"/>
+      <c r="C49" s="61"/>
+      <c r="D49" s="61"/>
+      <c r="E49" s="61"/>
+      <c r="F49" s="61"/>
+      <c r="G49" s="61"/>
       <c r="H49" s="7"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
-      <c r="B50" s="70"/>
-      <c r="C50" s="70"/>
-      <c r="D50" s="70"/>
-      <c r="E50" s="70"/>
-      <c r="F50" s="70"/>
-      <c r="G50" s="70"/>
+      <c r="B50" s="61"/>
+      <c r="C50" s="61"/>
+      <c r="D50" s="61"/>
+      <c r="E50" s="61"/>
+      <c r="F50" s="61"/>
+      <c r="G50" s="61"/>
       <c r="H50" s="7"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
-      <c r="B51" s="70"/>
-      <c r="C51" s="70"/>
-      <c r="D51" s="70"/>
-      <c r="E51" s="70"/>
-      <c r="F51" s="70"/>
-      <c r="G51" s="70"/>
+      <c r="B51" s="61"/>
+      <c r="C51" s="61"/>
+      <c r="D51" s="61"/>
+      <c r="E51" s="61"/>
+      <c r="F51" s="61"/>
+      <c r="G51" s="61"/>
       <c r="H51" s="7"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
-      <c r="B52" s="70"/>
-      <c r="C52" s="70"/>
-      <c r="D52" s="70"/>
-      <c r="E52" s="70"/>
-      <c r="F52" s="70"/>
-      <c r="G52" s="70"/>
+      <c r="B52" s="61"/>
+      <c r="C52" s="61"/>
+      <c r="D52" s="61"/>
+      <c r="E52" s="61"/>
+      <c r="F52" s="61"/>
+      <c r="G52" s="61"/>
       <c r="H52" s="7"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
-      <c r="B53" s="70"/>
-      <c r="C53" s="70"/>
-      <c r="D53" s="70"/>
-      <c r="E53" s="70"/>
-      <c r="F53" s="70"/>
-      <c r="G53" s="70"/>
+      <c r="B53" s="61"/>
+      <c r="C53" s="61"/>
+      <c r="D53" s="61"/>
+      <c r="E53" s="61"/>
+      <c r="F53" s="61"/>
+      <c r="G53" s="61"/>
       <c r="H53" s="7"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
-      <c r="B54" s="70"/>
-      <c r="C54" s="70"/>
-      <c r="D54" s="70"/>
-      <c r="E54" s="70"/>
-      <c r="F54" s="70"/>
-      <c r="G54" s="70"/>
+      <c r="B54" s="61"/>
+      <c r="C54" s="61"/>
+      <c r="D54" s="61"/>
+      <c r="E54" s="61"/>
+      <c r="F54" s="61"/>
+      <c r="G54" s="61"/>
       <c r="H54" s="7"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
-      <c r="B55" s="70"/>
-      <c r="C55" s="70"/>
-      <c r="D55" s="70"/>
-      <c r="E55" s="70"/>
-      <c r="F55" s="70"/>
-      <c r="G55" s="70"/>
+      <c r="B55" s="61"/>
+      <c r="C55" s="61"/>
+      <c r="D55" s="61"/>
+      <c r="E55" s="61"/>
+      <c r="F55" s="61"/>
+      <c r="G55" s="61"/>
       <c r="H55" s="7"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
-      <c r="B56" s="70"/>
-      <c r="C56" s="70"/>
-      <c r="D56" s="70"/>
-      <c r="E56" s="70"/>
-      <c r="F56" s="70"/>
-      <c r="G56" s="70"/>
+      <c r="B56" s="61"/>
+      <c r="C56" s="61"/>
+      <c r="D56" s="61"/>
+      <c r="E56" s="61"/>
+      <c r="F56" s="61"/>
+      <c r="G56" s="61"/>
       <c r="H56" s="7"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
-      <c r="B57" s="70"/>
-      <c r="C57" s="70"/>
-      <c r="D57" s="70"/>
-      <c r="E57" s="70"/>
-      <c r="F57" s="70"/>
-      <c r="G57" s="70"/>
+      <c r="B57" s="61"/>
+      <c r="C57" s="61"/>
+      <c r="D57" s="61"/>
+      <c r="E57" s="61"/>
+      <c r="F57" s="61"/>
+      <c r="G57" s="61"/>
       <c r="H57" s="7"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
-      <c r="B58" s="70"/>
-      <c r="C58" s="70"/>
-      <c r="D58" s="70"/>
-      <c r="E58" s="70"/>
-      <c r="F58" s="70"/>
-      <c r="G58" s="70"/>
+      <c r="B58" s="61"/>
+      <c r="C58" s="61"/>
+      <c r="D58" s="61"/>
+      <c r="E58" s="61"/>
+      <c r="F58" s="61"/>
+      <c r="G58" s="61"/>
       <c r="H58" s="7"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
-      <c r="B59" s="70"/>
-      <c r="C59" s="70"/>
-      <c r="D59" s="70"/>
-      <c r="E59" s="70"/>
-      <c r="F59" s="70"/>
-      <c r="G59" s="70"/>
+      <c r="B59" s="61"/>
+      <c r="C59" s="61"/>
+      <c r="D59" s="61"/>
+      <c r="E59" s="61"/>
+      <c r="F59" s="61"/>
+      <c r="G59" s="61"/>
       <c r="H59" s="7"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
-      <c r="B60" s="70"/>
-      <c r="C60" s="70"/>
-      <c r="D60" s="70"/>
-      <c r="E60" s="70"/>
-      <c r="F60" s="70"/>
-      <c r="G60" s="70"/>
+      <c r="B60" s="61"/>
+      <c r="C60" s="61"/>
+      <c r="D60" s="61"/>
+      <c r="E60" s="61"/>
+      <c r="F60" s="61"/>
+      <c r="G60" s="61"/>
       <c r="H60" s="7"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
-      <c r="B61" s="70"/>
-      <c r="C61" s="70"/>
-      <c r="D61" s="70"/>
-      <c r="E61" s="70"/>
-      <c r="F61" s="70"/>
-      <c r="G61" s="70"/>
+      <c r="B61" s="61"/>
+      <c r="C61" s="61"/>
+      <c r="D61" s="61"/>
+      <c r="E61" s="61"/>
+      <c r="F61" s="61"/>
+      <c r="G61" s="61"/>
       <c r="H61" s="7"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -11404,6 +11495,21 @@
     <row r="108" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B35:G61"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
     <mergeCell ref="B18:G18"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="B7:G7"/>
@@ -11416,21 +11522,6 @@
     <mergeCell ref="B15:G15"/>
     <mergeCell ref="B16:G16"/>
     <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:G61"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="C31:G31"/>
   </mergeCells>
   <conditionalFormatting sqref="G8">
     <cfRule type="iconSet" priority="1">
@@ -11489,11 +11580,11 @@
     <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -11531,14 +11622,14 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
@@ -11568,14 +11659,14 @@
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="59" t="str">
+      <c r="C9" s="70" t="str">
         <f>'TAREAS PROYECTO'!B15</f>
         <v>Seguridad</v>
       </c>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -11583,189 +11674,189 @@
       <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="58" t="str">
+      <c r="C10" s="69" t="str">
         <f>'TAREAS PROYECTO'!C15</f>
         <v>Opciones habilitadas</v>
       </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="61" t="s">
+      <c r="B12" s="59" t="s">
         <v>135</v>
       </c>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
       <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="59" t="s">
         <v>136</v>
       </c>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
-      <c r="B18" s="61"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="61"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="61"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59"/>
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="60"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
       <c r="H19" s="7"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
-      <c r="B20" s="62"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
-      <c r="G20" s="64"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="65"/>
       <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
-      <c r="B21" s="62"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63"/>
-      <c r="G21" s="64"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="65"/>
       <c r="H21" s="7"/>
     </row>
     <row r="22" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="62"/>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="64"/>
+      <c r="B22" s="63"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="65"/>
     </row>
     <row r="23" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="60" t="s">
+      <c r="B23" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="60"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
     </row>
     <row r="24" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="62" t="s">
+      <c r="C24" s="63" t="s">
         <v>132</v>
       </c>
-      <c r="D24" s="63"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="63"/>
-      <c r="G24" s="64"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="65"/>
     </row>
     <row r="25" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="65" t="s">
+      <c r="C25" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="D25" s="66"/>
-      <c r="E25" s="66"/>
-      <c r="F25" s="66"/>
-      <c r="G25" s="67"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="68"/>
     </row>
     <row r="26" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="62" t="s">
+      <c r="C26" s="63" t="s">
         <v>134</v>
       </c>
-      <c r="D26" s="63"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="63"/>
-      <c r="G26" s="64"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="64"/>
+      <c r="G26" s="65"/>
     </row>
     <row r="27" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
@@ -11784,14 +11875,14 @@
       <c r="G28" s="16"/>
     </row>
     <row r="29" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="60" t="s">
+      <c r="B29" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="C29" s="60"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="60"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="62"/>
     </row>
     <row r="30" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="71"/>
@@ -12216,12 +12307,13 @@
     <row r="110" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:J63"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
     <mergeCell ref="B19:G19"/>
     <mergeCell ref="B20:G20"/>
     <mergeCell ref="B21:G21"/>
@@ -12231,13 +12323,12 @@
     <mergeCell ref="B16:G16"/>
     <mergeCell ref="B17:G17"/>
     <mergeCell ref="B18:G18"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:J63"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="B11:G11"/>
   </mergeCells>
   <conditionalFormatting sqref="G8">
     <cfRule type="iconSet" priority="1">
@@ -12298,11 +12389,11 @@
     <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -12340,14 +12431,14 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
@@ -12377,14 +12468,14 @@
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="59" t="str">
+      <c r="C9" s="70" t="str">
         <f>'TAREAS PROYECTO'!B24</f>
         <v>Cargue informacion</v>
       </c>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -12392,214 +12483,214 @@
       <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="58" t="str">
+      <c r="C10" s="69" t="str">
         <f>'TAREAS PROYECTO'!C24</f>
         <v>Procesar cargue de archivos</v>
       </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="61" t="s">
+      <c r="B12" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
-      <c r="B13" s="61" t="s">
+      <c r="B13" s="59" t="s">
         <v>127</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
       <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="59" t="s">
         <v>128</v>
       </c>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
-      <c r="B18" s="61"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="61"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="61"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59"/>
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="60"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
       <c r="H19" s="7"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
-      <c r="B20" s="62" t="s">
+      <c r="B20" s="63" t="s">
         <v>129</v>
       </c>
-      <c r="C20" s="63"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
-      <c r="G20" s="64"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="65"/>
       <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
-      <c r="B21" s="62" t="s">
+      <c r="B21" s="63" t="s">
         <v>130</v>
       </c>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63"/>
-      <c r="G21" s="64"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="65"/>
       <c r="H21" s="7"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
-      <c r="B22" s="62" t="s">
+      <c r="B22" s="63" t="s">
         <v>131</v>
       </c>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="64"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="65"/>
       <c r="H22" s="7"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
-      <c r="B23" s="62"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63"/>
-      <c r="G23" s="64"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="65"/>
       <c r="H23" s="7"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
-      <c r="B24" s="62"/>
-      <c r="C24" s="63"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="63"/>
-      <c r="G24" s="64"/>
+      <c r="B24" s="63"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="65"/>
       <c r="H24" s="7"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="61"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
       <c r="H25" s="7"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
-      <c r="B26" s="62"/>
-      <c r="C26" s="63"/>
-      <c r="D26" s="63"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="63"/>
-      <c r="G26" s="64"/>
+      <c r="B26" s="63"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="64"/>
+      <c r="G26" s="65"/>
       <c r="H26" s="7"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
-      <c r="B27" s="62"/>
-      <c r="C27" s="63"/>
-      <c r="D27" s="63"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="64"/>
+      <c r="B27" s="63"/>
+      <c r="C27" s="64"/>
+      <c r="D27" s="64"/>
+      <c r="E27" s="64"/>
+      <c r="F27" s="64"/>
+      <c r="G27" s="65"/>
       <c r="H27" s="7"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
-      <c r="B28" s="60" t="s">
+      <c r="B28" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="60"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="60"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="62"/>
       <c r="H28" s="7"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -12607,13 +12698,13 @@
       <c r="B29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="62" t="s">
+      <c r="C29" s="63" t="s">
         <v>132</v>
       </c>
-      <c r="D29" s="63"/>
-      <c r="E29" s="63"/>
-      <c r="F29" s="63"/>
-      <c r="G29" s="64"/>
+      <c r="D29" s="64"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="64"/>
+      <c r="G29" s="65"/>
       <c r="H29" s="7"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -12621,13 +12712,13 @@
       <c r="B30" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="65" t="s">
+      <c r="C30" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="D30" s="66"/>
-      <c r="E30" s="66"/>
-      <c r="F30" s="66"/>
-      <c r="G30" s="67"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="68"/>
       <c r="H30" s="7"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -12635,13 +12726,13 @@
       <c r="B31" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="62" t="s">
+      <c r="C31" s="63" t="s">
         <v>134</v>
       </c>
-      <c r="D31" s="63"/>
-      <c r="E31" s="63"/>
-      <c r="F31" s="63"/>
-      <c r="G31" s="64"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="65"/>
       <c r="H31" s="7"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -12666,14 +12757,14 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
-      <c r="B34" s="60" t="s">
+      <c r="B34" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="C34" s="60"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="60"/>
-      <c r="F34" s="60"/>
-      <c r="G34" s="60"/>
+      <c r="C34" s="62"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="62"/>
+      <c r="F34" s="62"/>
+      <c r="G34" s="62"/>
       <c r="H34" s="7"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -13086,14 +13177,14 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
-      <c r="B69" s="60" t="s">
+      <c r="B69" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="C69" s="60"/>
-      <c r="D69" s="60"/>
-      <c r="E69" s="60"/>
-      <c r="F69" s="60"/>
-      <c r="G69" s="60"/>
+      <c r="C69" s="62"/>
+      <c r="D69" s="62"/>
+      <c r="E69" s="62"/>
+      <c r="F69" s="62"/>
+      <c r="G69" s="62"/>
       <c r="H69" s="7"/>
     </row>
     <row r="70" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -13151,6 +13242,18 @@
     <row r="115" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B35:J68"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="B34:G34"/>
     <mergeCell ref="B12:G12"/>
     <mergeCell ref="B69:G69"/>
     <mergeCell ref="C3:E3"/>
@@ -13167,18 +13270,6 @@
     <mergeCell ref="B18:G18"/>
     <mergeCell ref="B19:G19"/>
     <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B35:J68"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
   </mergeCells>
   <conditionalFormatting sqref="G8">
     <cfRule type="iconSet" priority="1">
@@ -13240,11 +13331,11 @@
     <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -13282,14 +13373,14 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
@@ -13319,14 +13410,14 @@
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="59" t="str">
+      <c r="C9" s="70" t="str">
         <f>'TAREAS PROYECTO'!B24</f>
         <v>Cargue informacion</v>
       </c>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -13334,171 +13425,171 @@
       <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="58" t="str">
+      <c r="C10" s="69" t="str">
         <f>'TAREAS ITERACION'!C25</f>
         <v>Edicion Recaudo local - transferencias</v>
       </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="61" t="s">
+      <c r="B12" s="59" t="s">
         <v>262</v>
       </c>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
       <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="59" t="s">
         <v>263</v>
       </c>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
-      <c r="B18" s="61"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="61"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="61"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59"/>
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="60"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
       <c r="H19" s="7"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
-      <c r="B20" s="62"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
-      <c r="G20" s="64"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="65"/>
       <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="60" t="s">
+      <c r="B21" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="60"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="60"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="62"/>
     </row>
     <row r="22" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="62" t="s">
+      <c r="C22" s="63" t="s">
         <v>265</v>
       </c>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="65"/>
     </row>
     <row r="23" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="65" t="s">
+      <c r="C23" s="66" t="s">
         <v>266</v>
       </c>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="68"/>
     </row>
     <row r="24" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="62" t="s">
-        <v>302</v>
-      </c>
-      <c r="D24" s="63"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="63"/>
-      <c r="G24" s="64"/>
+      <c r="C24" s="63" t="s">
+        <v>301</v>
+      </c>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="65"/>
     </row>
     <row r="25" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
@@ -13512,37 +13603,37 @@
       <c r="B26" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="62" t="s">
+      <c r="C26" s="63" t="s">
         <v>267</v>
       </c>
-      <c r="D26" s="63"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="63"/>
-      <c r="G26" s="64"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="64"/>
+      <c r="G26" s="65"/>
     </row>
     <row r="27" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="65" t="s">
+      <c r="C27" s="66" t="s">
         <v>268</v>
       </c>
-      <c r="D27" s="66"/>
-      <c r="E27" s="66"/>
-      <c r="F27" s="66"/>
-      <c r="G27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="68"/>
     </row>
     <row r="28" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="62" t="s">
+      <c r="C28" s="63" t="s">
         <v>269</v>
       </c>
-      <c r="D28" s="63"/>
-      <c r="E28" s="63"/>
-      <c r="F28" s="63"/>
-      <c r="G28" s="64"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="64"/>
+      <c r="F28" s="64"/>
+      <c r="G28" s="65"/>
     </row>
     <row r="29" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
@@ -13556,37 +13647,37 @@
       <c r="B30" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="62" t="s">
+      <c r="C30" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="D30" s="63"/>
-      <c r="E30" s="63"/>
-      <c r="F30" s="63"/>
-      <c r="G30" s="64"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="64"/>
+      <c r="G30" s="65"/>
     </row>
     <row r="31" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="65" t="s">
+      <c r="C31" s="66" t="s">
         <v>271</v>
       </c>
-      <c r="D31" s="66"/>
-      <c r="E31" s="66"/>
-      <c r="F31" s="66"/>
-      <c r="G31" s="67"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="68"/>
     </row>
     <row r="32" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="62" t="s">
+      <c r="C32" s="63" t="s">
         <v>272</v>
       </c>
-      <c r="D32" s="63"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="63"/>
-      <c r="G32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="64"/>
+      <c r="G32" s="65"/>
     </row>
     <row r="33" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
@@ -13610,37 +13701,37 @@
       <c r="B35" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="62" t="s">
+      <c r="C35" s="63" t="s">
         <v>270</v>
       </c>
-      <c r="D35" s="63"/>
-      <c r="E35" s="63"/>
-      <c r="F35" s="63"/>
-      <c r="G35" s="64"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="64"/>
+      <c r="G35" s="65"/>
     </row>
     <row r="36" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="65" t="s">
+      <c r="C36" s="66" t="s">
         <v>274</v>
       </c>
-      <c r="D36" s="66"/>
-      <c r="E36" s="66"/>
-      <c r="F36" s="66"/>
-      <c r="G36" s="67"/>
+      <c r="D36" s="67"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="68"/>
     </row>
     <row r="37" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="62" t="s">
+      <c r="C37" s="63" t="s">
         <v>275</v>
       </c>
-      <c r="D37" s="63"/>
-      <c r="E37" s="63"/>
-      <c r="F37" s="63"/>
-      <c r="G37" s="64"/>
+      <c r="D37" s="64"/>
+      <c r="E37" s="64"/>
+      <c r="F37" s="64"/>
+      <c r="G37" s="65"/>
     </row>
     <row r="38" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="5"/>
@@ -13693,14 +13784,14 @@
       <c r="G43" s="21"/>
     </row>
     <row r="44" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="60" t="s">
+      <c r="B44" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="C44" s="60"/>
-      <c r="D44" s="60"/>
-      <c r="E44" s="60"/>
-      <c r="F44" s="60"/>
-      <c r="G44" s="60"/>
+      <c r="C44" s="62"/>
+      <c r="D44" s="62"/>
+      <c r="E44" s="62"/>
+      <c r="F44" s="62"/>
+      <c r="G44" s="62"/>
     </row>
     <row r="45" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="50"/>
@@ -14188,7 +14279,7 @@
       <c r="I88" s="51"/>
       <c r="J88" s="51"/>
       <c r="K88" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="89" spans="2:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -14302,14 +14393,14 @@
       <c r="J98" s="51"/>
     </row>
     <row r="99" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="60" t="s">
+      <c r="B99" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="C99" s="60"/>
-      <c r="D99" s="60"/>
-      <c r="E99" s="60"/>
-      <c r="F99" s="60"/>
-      <c r="G99" s="60"/>
+      <c r="C99" s="62"/>
+      <c r="D99" s="62"/>
+      <c r="E99" s="62"/>
+      <c r="F99" s="62"/>
+      <c r="G99" s="62"/>
     </row>
     <row r="100" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B100" s="7" t="s">
@@ -14374,23 +14465,6 @@
     <row r="145" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B20:G20"/>
     <mergeCell ref="C24:G24"/>
     <mergeCell ref="B44:G44"/>
     <mergeCell ref="B99:G99"/>
@@ -14404,6 +14478,23 @@
     <mergeCell ref="C35:G35"/>
     <mergeCell ref="C36:G36"/>
     <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
   </mergeCells>
   <conditionalFormatting sqref="G8">
     <cfRule type="iconSet" priority="1">
@@ -14468,11 +14559,11 @@
     <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -14510,14 +14601,14 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
@@ -14547,14 +14638,14 @@
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="59" t="str">
+      <c r="C9" s="70" t="str">
         <f>'TAREAS PROYECTO'!B76</f>
         <v>Seguridad</v>
       </c>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -14562,181 +14653,181 @@
       <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="58" t="str">
+      <c r="C10" s="69" t="str">
         <f>'TAREAS PROYECTO'!C76</f>
         <v>Cerrar sesion</v>
       </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="61" t="s">
+      <c r="B12" s="59" t="s">
         <v>138</v>
       </c>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
       <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="59" t="s">
         <v>137</v>
       </c>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
-      <c r="B18" s="61"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="61"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="61"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59"/>
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="60"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
       <c r="H19" s="7"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
-      <c r="B20" s="62" t="s">
+      <c r="B20" s="63" t="s">
         <v>139</v>
       </c>
-      <c r="C20" s="63"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
-      <c r="G20" s="64"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="65"/>
       <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="62"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63"/>
-      <c r="G21" s="64"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="65"/>
     </row>
     <row r="22" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="60" t="s">
+      <c r="B22" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="60"/>
-      <c r="G22" s="60"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="62"/>
     </row>
     <row r="23" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="62" t="s">
+      <c r="C23" s="63" t="s">
         <v>140</v>
       </c>
-      <c r="D23" s="63"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63"/>
-      <c r="G23" s="64"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="65"/>
     </row>
     <row r="24" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="65" t="s">
+      <c r="C24" s="66" t="s">
         <v>141</v>
       </c>
-      <c r="D24" s="66"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="67"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="68"/>
     </row>
     <row r="25" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="62" t="s">
+      <c r="C25" s="63" t="s">
         <v>142</v>
       </c>
-      <c r="D25" s="63"/>
-      <c r="E25" s="63"/>
-      <c r="F25" s="63"/>
-      <c r="G25" s="64"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="64"/>
+      <c r="G25" s="65"/>
     </row>
     <row r="26" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
@@ -14755,230 +14846,230 @@
       <c r="G27" s="16"/>
     </row>
     <row r="28" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="60" t="s">
+      <c r="B28" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="C28" s="60"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="60"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="62"/>
     </row>
     <row r="29" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="70"/>
-      <c r="C29" s="70"/>
-      <c r="D29" s="70"/>
-      <c r="E29" s="70"/>
-      <c r="F29" s="70"/>
-      <c r="G29" s="70"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="61"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="61"/>
+      <c r="G29" s="61"/>
     </row>
     <row r="30" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="70"/>
-      <c r="C30" s="70"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="70"/>
-      <c r="F30" s="70"/>
-      <c r="G30" s="70"/>
+      <c r="B30" s="61"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="61"/>
+      <c r="E30" s="61"/>
+      <c r="F30" s="61"/>
+      <c r="G30" s="61"/>
     </row>
     <row r="31" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="70"/>
-      <c r="C31" s="70"/>
-      <c r="D31" s="70"/>
-      <c r="E31" s="70"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="70"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="61"/>
+      <c r="G31" s="61"/>
     </row>
     <row r="32" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="70"/>
-      <c r="C32" s="70"/>
-      <c r="D32" s="70"/>
-      <c r="E32" s="70"/>
-      <c r="F32" s="70"/>
-      <c r="G32" s="70"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="61"/>
+      <c r="G32" s="61"/>
     </row>
     <row r="33" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="70"/>
-      <c r="C33" s="70"/>
-      <c r="D33" s="70"/>
-      <c r="E33" s="70"/>
-      <c r="F33" s="70"/>
-      <c r="G33" s="70"/>
+      <c r="B33" s="61"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="61"/>
     </row>
     <row r="34" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="70"/>
-      <c r="C34" s="70"/>
-      <c r="D34" s="70"/>
-      <c r="E34" s="70"/>
-      <c r="F34" s="70"/>
-      <c r="G34" s="70"/>
+      <c r="B34" s="61"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="61"/>
+      <c r="G34" s="61"/>
     </row>
     <row r="35" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="70"/>
-      <c r="C35" s="70"/>
-      <c r="D35" s="70"/>
-      <c r="E35" s="70"/>
-      <c r="F35" s="70"/>
-      <c r="G35" s="70"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="61"/>
     </row>
     <row r="36" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="70"/>
-      <c r="C36" s="70"/>
-      <c r="D36" s="70"/>
-      <c r="E36" s="70"/>
-      <c r="F36" s="70"/>
-      <c r="G36" s="70"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="61"/>
+      <c r="F36" s="61"/>
+      <c r="G36" s="61"/>
     </row>
     <row r="37" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="70"/>
-      <c r="C37" s="70"/>
-      <c r="D37" s="70"/>
-      <c r="E37" s="70"/>
-      <c r="F37" s="70"/>
-      <c r="G37" s="70"/>
+      <c r="B37" s="61"/>
+      <c r="C37" s="61"/>
+      <c r="D37" s="61"/>
+      <c r="E37" s="61"/>
+      <c r="F37" s="61"/>
+      <c r="G37" s="61"/>
     </row>
     <row r="38" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="70"/>
-      <c r="C38" s="70"/>
-      <c r="D38" s="70"/>
-      <c r="E38" s="70"/>
-      <c r="F38" s="70"/>
-      <c r="G38" s="70"/>
+      <c r="B38" s="61"/>
+      <c r="C38" s="61"/>
+      <c r="D38" s="61"/>
+      <c r="E38" s="61"/>
+      <c r="F38" s="61"/>
+      <c r="G38" s="61"/>
     </row>
     <row r="39" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="70"/>
-      <c r="C39" s="70"/>
-      <c r="D39" s="70"/>
-      <c r="E39" s="70"/>
-      <c r="F39" s="70"/>
-      <c r="G39" s="70"/>
+      <c r="B39" s="61"/>
+      <c r="C39" s="61"/>
+      <c r="D39" s="61"/>
+      <c r="E39" s="61"/>
+      <c r="F39" s="61"/>
+      <c r="G39" s="61"/>
     </row>
     <row r="40" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="70"/>
-      <c r="C40" s="70"/>
-      <c r="D40" s="70"/>
-      <c r="E40" s="70"/>
-      <c r="F40" s="70"/>
-      <c r="G40" s="70"/>
+      <c r="B40" s="61"/>
+      <c r="C40" s="61"/>
+      <c r="D40" s="61"/>
+      <c r="E40" s="61"/>
+      <c r="F40" s="61"/>
+      <c r="G40" s="61"/>
     </row>
     <row r="41" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="70"/>
-      <c r="C41" s="70"/>
-      <c r="D41" s="70"/>
-      <c r="E41" s="70"/>
-      <c r="F41" s="70"/>
-      <c r="G41" s="70"/>
+      <c r="B41" s="61"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="61"/>
+      <c r="E41" s="61"/>
+      <c r="F41" s="61"/>
+      <c r="G41" s="61"/>
     </row>
     <row r="42" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="70"/>
-      <c r="C42" s="70"/>
-      <c r="D42" s="70"/>
-      <c r="E42" s="70"/>
-      <c r="F42" s="70"/>
-      <c r="G42" s="70"/>
+      <c r="B42" s="61"/>
+      <c r="C42" s="61"/>
+      <c r="D42" s="61"/>
+      <c r="E42" s="61"/>
+      <c r="F42" s="61"/>
+      <c r="G42" s="61"/>
     </row>
     <row r="43" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="70"/>
-      <c r="C43" s="70"/>
-      <c r="D43" s="70"/>
-      <c r="E43" s="70"/>
-      <c r="F43" s="70"/>
-      <c r="G43" s="70"/>
+      <c r="B43" s="61"/>
+      <c r="C43" s="61"/>
+      <c r="D43" s="61"/>
+      <c r="E43" s="61"/>
+      <c r="F43" s="61"/>
+      <c r="G43" s="61"/>
     </row>
     <row r="44" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="70"/>
-      <c r="C44" s="70"/>
-      <c r="D44" s="70"/>
-      <c r="E44" s="70"/>
-      <c r="F44" s="70"/>
-      <c r="G44" s="70"/>
+      <c r="B44" s="61"/>
+      <c r="C44" s="61"/>
+      <c r="D44" s="61"/>
+      <c r="E44" s="61"/>
+      <c r="F44" s="61"/>
+      <c r="G44" s="61"/>
     </row>
     <row r="45" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="70"/>
-      <c r="C45" s="70"/>
-      <c r="D45" s="70"/>
-      <c r="E45" s="70"/>
-      <c r="F45" s="70"/>
-      <c r="G45" s="70"/>
+      <c r="B45" s="61"/>
+      <c r="C45" s="61"/>
+      <c r="D45" s="61"/>
+      <c r="E45" s="61"/>
+      <c r="F45" s="61"/>
+      <c r="G45" s="61"/>
     </row>
     <row r="46" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="70"/>
-      <c r="C46" s="70"/>
-      <c r="D46" s="70"/>
-      <c r="E46" s="70"/>
-      <c r="F46" s="70"/>
-      <c r="G46" s="70"/>
+      <c r="B46" s="61"/>
+      <c r="C46" s="61"/>
+      <c r="D46" s="61"/>
+      <c r="E46" s="61"/>
+      <c r="F46" s="61"/>
+      <c r="G46" s="61"/>
     </row>
     <row r="47" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="70"/>
-      <c r="C47" s="70"/>
-      <c r="D47" s="70"/>
-      <c r="E47" s="70"/>
-      <c r="F47" s="70"/>
-      <c r="G47" s="70"/>
+      <c r="B47" s="61"/>
+      <c r="C47" s="61"/>
+      <c r="D47" s="61"/>
+      <c r="E47" s="61"/>
+      <c r="F47" s="61"/>
+      <c r="G47" s="61"/>
     </row>
     <row r="48" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="70"/>
-      <c r="C48" s="70"/>
-      <c r="D48" s="70"/>
-      <c r="E48" s="70"/>
-      <c r="F48" s="70"/>
-      <c r="G48" s="70"/>
+      <c r="B48" s="61"/>
+      <c r="C48" s="61"/>
+      <c r="D48" s="61"/>
+      <c r="E48" s="61"/>
+      <c r="F48" s="61"/>
+      <c r="G48" s="61"/>
     </row>
     <row r="49" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="70"/>
-      <c r="C49" s="70"/>
-      <c r="D49" s="70"/>
-      <c r="E49" s="70"/>
-      <c r="F49" s="70"/>
-      <c r="G49" s="70"/>
+      <c r="B49" s="61"/>
+      <c r="C49" s="61"/>
+      <c r="D49" s="61"/>
+      <c r="E49" s="61"/>
+      <c r="F49" s="61"/>
+      <c r="G49" s="61"/>
     </row>
     <row r="50" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="70"/>
-      <c r="C50" s="70"/>
-      <c r="D50" s="70"/>
-      <c r="E50" s="70"/>
-      <c r="F50" s="70"/>
-      <c r="G50" s="70"/>
+      <c r="B50" s="61"/>
+      <c r="C50" s="61"/>
+      <c r="D50" s="61"/>
+      <c r="E50" s="61"/>
+      <c r="F50" s="61"/>
+      <c r="G50" s="61"/>
     </row>
     <row r="51" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="70"/>
-      <c r="C51" s="70"/>
-      <c r="D51" s="70"/>
-      <c r="E51" s="70"/>
-      <c r="F51" s="70"/>
-      <c r="G51" s="70"/>
+      <c r="B51" s="61"/>
+      <c r="C51" s="61"/>
+      <c r="D51" s="61"/>
+      <c r="E51" s="61"/>
+      <c r="F51" s="61"/>
+      <c r="G51" s="61"/>
     </row>
     <row r="52" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="70"/>
-      <c r="C52" s="70"/>
-      <c r="D52" s="70"/>
-      <c r="E52" s="70"/>
-      <c r="F52" s="70"/>
-      <c r="G52" s="70"/>
+      <c r="B52" s="61"/>
+      <c r="C52" s="61"/>
+      <c r="D52" s="61"/>
+      <c r="E52" s="61"/>
+      <c r="F52" s="61"/>
+      <c r="G52" s="61"/>
     </row>
     <row r="53" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="70"/>
-      <c r="C53" s="70"/>
-      <c r="D53" s="70"/>
-      <c r="E53" s="70"/>
-      <c r="F53" s="70"/>
-      <c r="G53" s="70"/>
+      <c r="B53" s="61"/>
+      <c r="C53" s="61"/>
+      <c r="D53" s="61"/>
+      <c r="E53" s="61"/>
+      <c r="F53" s="61"/>
+      <c r="G53" s="61"/>
     </row>
     <row r="54" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="70"/>
-      <c r="C54" s="70"/>
-      <c r="D54" s="70"/>
-      <c r="E54" s="70"/>
-      <c r="F54" s="70"/>
-      <c r="G54" s="70"/>
+      <c r="B54" s="61"/>
+      <c r="C54" s="61"/>
+      <c r="D54" s="61"/>
+      <c r="E54" s="61"/>
+      <c r="F54" s="61"/>
+      <c r="G54" s="61"/>
     </row>
     <row r="55" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="70"/>
-      <c r="C55" s="70"/>
-      <c r="D55" s="70"/>
-      <c r="E55" s="70"/>
-      <c r="F55" s="70"/>
-      <c r="G55" s="70"/>
+      <c r="B55" s="61"/>
+      <c r="C55" s="61"/>
+      <c r="D55" s="61"/>
+      <c r="E55" s="61"/>
+      <c r="F55" s="61"/>
+      <c r="G55" s="61"/>
     </row>
     <row r="56" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -15029,12 +15120,13 @@
     <row r="102" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B29:G55"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
     <mergeCell ref="B19:G19"/>
     <mergeCell ref="B20:G20"/>
     <mergeCell ref="B13:G13"/>
@@ -15043,13 +15135,12 @@
     <mergeCell ref="B16:G16"/>
     <mergeCell ref="B17:G17"/>
     <mergeCell ref="B18:G18"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B29:G55"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="B11:G11"/>
   </mergeCells>
   <conditionalFormatting sqref="G8">
     <cfRule type="iconSet" priority="1">

</xml_diff>

<commit_message>
Se incluye servicio editarTransferencia
</commit_message>
<xml_diff>
--- a/Sevial/Sevial.DOC/Requerimientos/Tareas y historias.xlsx
+++ b/Sevial/Sevial.DOC/Requerimientos/Tareas y historias.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6585" firstSheet="8" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6585" firstSheet="9" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="TAREAS PROYECTO" sheetId="2" r:id="rId1"/>
@@ -1126,7 +1126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="345">
   <si>
     <t>ID</t>
   </si>
@@ -2019,12 +2019,6 @@
     <t>observacion</t>
   </si>
   <si>
-    <t>banco</t>
-  </si>
-  <si>
-    <t>cuenta</t>
-  </si>
-  <si>
     <t>idRegistroTrf</t>
   </si>
   <si>
@@ -2040,21 +2034,12 @@
     <t>id del registro a eliminar</t>
   </si>
   <si>
-    <t>cargueInformacion/editarTransferencia</t>
-  </si>
-  <si>
     <t>Permite actualizar o crear una transferencia</t>
   </si>
   <si>
     <t>Fecha en formato aaaa-mm-dd</t>
   </si>
   <si>
-    <t>Nombre banco</t>
-  </si>
-  <si>
-    <t>Numero cuenta</t>
-  </si>
-  <si>
     <t>identificador unico del registro (0 si es nuevo)</t>
   </si>
   <si>
@@ -2122,6 +2107,61 @@
   </si>
   <si>
     <t>idRegistro</t>
+  </si>
+  <si>
+    <t>informacion/editarTransferencia</t>
+  </si>
+  <si>
+    <t>idEstadoGestion</t>
+  </si>
+  <si>
+    <t>idCuantia</t>
+  </si>
+  <si>
+    <t>vlrTrf45</t>
+  </si>
+  <si>
+    <t>vlrTrf10</t>
+  </si>
+  <si>
+    <t>Año inicial - Año Final (aaaa-aaaa)</t>
+  </si>
+  <si>
+    <t>valores de la categoria ESTADO_GESTION</t>
+  </si>
+  <si>
+    <t>valores de categoria MUNICIPIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valores de la categoria CUANTIA
+</t>
+  </si>
+  <si>
+    <t>valores de la categoria TIPO_TRANSFERENCIA</t>
+  </si>
+  <si>
+    <t>idTipoTrf</t>
+  </si>
+  <si>
+    <t>idBancoCuenta</t>
+  </si>
+  <si>
+    <t>valores de la categoria BANCO_CUENTA</t>
+  </si>
+  <si>
+    <t>bancoCuenta</t>
+  </si>
+  <si>
+    <t>Nombre banco -cuenta</t>
+  </si>
+  <si>
+    <t>idAutoridadImposicion</t>
+  </si>
+  <si>
+    <t>Autoridad de imposicion</t>
+  </si>
+  <si>
+    <t>valores de la categoria AUTORIDAD_IMPOSICION</t>
   </si>
 </sst>
 </file>
@@ -3030,18 +3070,18 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>46759</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>8524</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>341902</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>122762</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3054,8 +3094,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="762000" y="7620000"/>
-          <a:ext cx="6923809" cy="8009524"/>
+          <a:off x="762000" y="7810500"/>
+          <a:ext cx="7980952" cy="8504762"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3099,6 +3139,49 @@
         <a:xfrm>
           <a:off x="762000" y="4000500"/>
           <a:ext cx="7228571" cy="5057143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>675331</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>84690</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="6858000"/>
+          <a:ext cx="7552381" cy="8276190"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7103,7 +7186,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -7370,7 +7453,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -7784,7 +7867,7 @@
         <v>229</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -7906,8 +7989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:G7"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7954,7 +8037,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -8086,10 +8169,10 @@
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="25"/>
       <c r="C18" s="23" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="E18" s="23"/>
       <c r="F18" s="23"/>
@@ -8101,7 +8184,7 @@
         <v>281</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="E19" s="23"/>
       <c r="F19" s="23"/>
@@ -8113,7 +8196,7 @@
         <v>282</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="E20" s="23"/>
       <c r="F20" s="23"/>
@@ -8125,7 +8208,7 @@
         <v>283</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="E21" s="23"/>
       <c r="F21" s="23"/>
@@ -8137,7 +8220,7 @@
         <v>284</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E22" s="23"/>
       <c r="F22" s="23"/>
@@ -8149,7 +8232,7 @@
         <v>285</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="E23" s="23"/>
       <c r="F23" s="23"/>
@@ -8161,7 +8244,7 @@
         <v>286</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E24" s="23"/>
       <c r="F24" s="23"/>
@@ -8173,7 +8256,7 @@
         <v>287</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="E25" s="23"/>
       <c r="F25" s="23"/>
@@ -8185,7 +8268,7 @@
         <v>288</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="E26" s="23"/>
       <c r="F26" s="23"/>
@@ -8197,7 +8280,7 @@
         <v>289</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="E27" s="23"/>
       <c r="F27" s="23"/>
@@ -8209,7 +8292,7 @@
         <v>290</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="E28" s="23"/>
       <c r="F28" s="23"/>
@@ -8221,7 +8304,7 @@
         <v>291</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="E29" s="23"/>
       <c r="F29" s="23"/>
@@ -8233,7 +8316,7 @@
         <v>292</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="E30" s="23"/>
       <c r="F30" s="23"/>
@@ -8245,7 +8328,7 @@
         <v>293</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="E31" s="23"/>
       <c r="F31" s="23"/>
@@ -8257,7 +8340,7 @@
         <v>294</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="E32" s="23"/>
       <c r="F32" s="23"/>
@@ -8269,7 +8352,7 @@
         <v>295</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="E33" s="23"/>
       <c r="F33" s="23"/>
@@ -8281,7 +8364,7 @@
         <v>296</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="E34" s="23"/>
       <c r="F34" s="23"/>
@@ -8290,10 +8373,10 @@
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="25"/>
       <c r="C35" s="23" t="s">
-        <v>297</v>
+        <v>340</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>307</v>
+        <v>341</v>
       </c>
       <c r="E35" s="23"/>
       <c r="F35" s="23"/>
@@ -8302,10 +8385,10 @@
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="25"/>
       <c r="C36" s="23" t="s">
-        <v>298</v>
+        <v>342</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>308</v>
+        <v>343</v>
       </c>
       <c r="E36" s="23"/>
       <c r="F36" s="23"/>
@@ -8354,7 +8437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -8402,7 +8485,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -8421,7 +8504,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="40" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -8461,10 +8544,10 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -8560,10 +8643,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G35"/>
+  <dimension ref="B3:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8610,7 +8693,7 @@
         <v>148</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>304</v>
+        <v>327</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
@@ -8629,7 +8712,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="40" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -8669,10 +8752,10 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="23"/>
@@ -8681,10 +8764,10 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>281</v>
+        <v>328</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>310</v>
+        <v>333</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="23"/>
@@ -8696,7 +8779,7 @@
         <v>284</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>300</v>
+        <v>334</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="23"/>
@@ -8708,7 +8791,7 @@
         <v>285</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="23"/>
@@ -8717,10 +8800,10 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="25" t="s">
-        <v>286</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>311</v>
+        <v>329</v>
+      </c>
+      <c r="C16" s="51" t="s">
+        <v>335</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="23"/>
@@ -8729,10 +8812,10 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
-        <v>287</v>
+        <v>330</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="23"/>
@@ -8741,10 +8824,10 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="25" t="s">
-        <v>288</v>
+        <v>331</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="23"/>
@@ -8756,7 +8839,7 @@
         <v>289</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="23"/>
@@ -8768,7 +8851,7 @@
         <v>290</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="23"/>
@@ -8780,7 +8863,7 @@
         <v>291</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>315</v>
+        <v>332</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="23"/>
@@ -8792,7 +8875,7 @@
         <v>292</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="23"/>
@@ -8804,7 +8887,7 @@
         <v>293</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="23"/>
@@ -8813,10 +8896,10 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
-        <v>294</v>
+        <v>337</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>318</v>
+        <v>336</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="23"/>
@@ -8825,10 +8908,10 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="25" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="23"/>
@@ -8837,10 +8920,10 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="25" t="s">
-        <v>296</v>
+        <v>338</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>317</v>
+        <v>339</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="23"/>
@@ -8849,10 +8932,10 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="25" t="s">
-        <v>297</v>
+        <v>342</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>307</v>
+        <v>344</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="23"/>
@@ -8860,108 +8943,97 @@
       <c r="G27" s="26"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="25" t="s">
-        <v>298</v>
-      </c>
-      <c r="C28" s="23" t="s">
-        <v>308</v>
-      </c>
-      <c r="D28" s="7"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
       <c r="E28" s="23"/>
       <c r="F28" s="23"/>
       <c r="G28" s="26"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="25"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="26"/>
+      <c r="B29" s="77" t="s">
+        <v>153</v>
+      </c>
+      <c r="C29" s="78"/>
+      <c r="D29" s="78"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="78"/>
+      <c r="G29" s="79"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="77" t="s">
-        <v>153</v>
-      </c>
-      <c r="C30" s="78"/>
-      <c r="D30" s="78"/>
-      <c r="E30" s="78"/>
-      <c r="F30" s="78"/>
-      <c r="G30" s="79"/>
+      <c r="B30" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="C30" s="23">
+        <v>0</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="26"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="25" t="s">
-        <v>154</v>
-      </c>
-      <c r="C31" s="23">
-        <v>0</v>
+      <c r="B31" s="25"/>
+      <c r="C31" s="42" t="s">
+        <v>182</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>214</v>
+        <v>183</v>
       </c>
       <c r="E31" s="23"/>
       <c r="F31" s="23"/>
       <c r="G31" s="26"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="25"/>
-      <c r="C32" s="42" t="s">
-        <v>182</v>
-      </c>
-      <c r="D32" s="23" t="s">
-        <v>183</v>
-      </c>
+      <c r="B32" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D32" s="23"/>
       <c r="E32" s="23"/>
       <c r="F32" s="23"/>
       <c r="G32" s="26"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="C33" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="26"/>
+      <c r="B33" s="77" t="s">
+        <v>170</v>
+      </c>
+      <c r="C33" s="78"/>
+      <c r="D33" s="78"/>
+      <c r="E33" s="78"/>
+      <c r="F33" s="78"/>
+      <c r="G33" s="79"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="77" t="s">
-        <v>170</v>
-      </c>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="78"/>
-      <c r="G34" s="79"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="32" t="s">
+      <c r="B34" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="C35" s="47">
+      <c r="C34" s="47">
         <v>25</v>
       </c>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="34"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B34:G34"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B33:G33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G4" location="SERVICIOS!A1" display="Lista Servicios"/>
-    <hyperlink ref="C35" location="'HISTORIA 25'!A1" display="'HISTORIA 25'!A1"/>
+    <hyperlink ref="C34" location="'HISTORIA 25'!A1" display="'HISTORIA 25'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9910,7 +9982,7 @@
       </c>
       <c r="B17" t="str">
         <f>'SERVICIO 10'!C6</f>
-        <v>cargueInformacion/editarTransferencia</v>
+        <v>informacion/editarTransferencia</v>
       </c>
       <c r="C17" s="36">
         <v>25</v>
@@ -9936,7 +10008,7 @@
         <v>Edicion Recaudo local - transferencias</v>
       </c>
       <c r="E18" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -9955,7 +10027,7 @@
         <v>Edicion Recaudo local - transferencias</v>
       </c>
       <c r="E19" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -9974,7 +10046,7 @@
         <v>Edicion Recaudo local - transferencias</v>
       </c>
       <c r="E20" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -9993,7 +10065,7 @@
         <v>Edicion Recaudo local - transferencias</v>
       </c>
       <c r="E21" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -12355,7 +12427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R115"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
@@ -13297,9 +13369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R145"/>
   <sheetViews>
-    <sheetView topLeftCell="C88" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
-    </sheetView>
+    <sheetView topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13584,7 +13654,7 @@
         <v>14</v>
       </c>
       <c r="C24" s="63" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D24" s="64"/>
       <c r="E24" s="64"/>
@@ -14279,7 +14349,7 @@
       <c r="I88" s="51"/>
       <c r="J88" s="51"/>
       <c r="K88" s="7" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="89" spans="2:11" s="7" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Servicios para Historia 75 - departamentales
</commit_message>
<xml_diff>
--- a/Sevial/Sevial.DOC/Requerimientos/Tareas y historias.xlsx
+++ b/Sevial/Sevial.DOC/Requerimientos/Tareas y historias.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="5670" firstSheet="28" activeTab="37"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="5670" firstSheet="14" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="TAREAS PROYECTO" sheetId="2" r:id="rId1"/>
@@ -50,6 +50,10 @@
     <sheet name="SERVICIO 15" sheetId="37" r:id="rId36"/>
     <sheet name="SERVICIO 16" sheetId="38" r:id="rId37"/>
     <sheet name="SERVICIO 17" sheetId="39" r:id="rId38"/>
+    <sheet name="SERVICIO 18" sheetId="40" r:id="rId39"/>
+    <sheet name="SERVICIO 19" sheetId="41" r:id="rId40"/>
+    <sheet name="SERVICIO 20" sheetId="42" r:id="rId41"/>
+    <sheet name="SERVICIO 21" sheetId="43" r:id="rId42"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'TAREAS ITERACION 1'!$A$8:$I$26</definedName>
@@ -2370,7 +2374,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="552">
   <si>
     <t>ID</t>
   </si>
@@ -3913,6 +3917,120 @@
   </si>
   <si>
     <t>Observacion sobre entrega</t>
+  </si>
+  <si>
+    <t>deuda/editarDetalleEntregaCartera</t>
+  </si>
+  <si>
+    <t>id del registro del detalle a editar</t>
+  </si>
+  <si>
+    <t>Fecha inical de entrega de cartera (aaaammdd)</t>
+  </si>
+  <si>
+    <t>Fecha final de entrega de cartera (aaaammdd)</t>
+  </si>
+  <si>
+    <t>estadoMunicipio</t>
+  </si>
+  <si>
+    <t>Estado de la entrega A:Activo I:Inactivo</t>
+  </si>
+  <si>
+    <t>Observacion a la entrega</t>
+  </si>
+  <si>
+    <t>editar el detalle de un a entrega a DITRA de un municipio especifico</t>
+  </si>
+  <si>
+    <t>Permitir ingresar nombre departamental</t>
+  </si>
+  <si>
+    <t>Permitir ingresar DIVIPOLA, debe ser de 8 caracteres numericos</t>
+  </si>
+  <si>
+    <t>Servicio</t>
+  </si>
+  <si>
+    <t>Valor categoria</t>
+  </si>
+  <si>
+    <t>Cuando es nuevo</t>
+  </si>
+  <si>
+    <t>Cuando se pase a la lista de municipios del departamental, agregar a  la lista de municipio departamental y eliminar de lista de municipios disponibles</t>
+  </si>
+  <si>
+    <t>La lista de municipios disponibles:</t>
+  </si>
+  <si>
+    <t>Cuando se guarde se envia lista de municipios departamental con su valor a011_codigo, separado por ;</t>
+  </si>
+  <si>
+    <t>Cuando se edita uno que existe</t>
+  </si>
+  <si>
+    <t>No se permite modificar el campo DIVIPOLA</t>
+  </si>
+  <si>
+    <t>parametro/listarDepartamentales</t>
+  </si>
+  <si>
+    <t>listar departamentales</t>
+  </si>
+  <si>
+    <t>A016_codigo</t>
+  </si>
+  <si>
+    <t>A016_nombre</t>
+  </si>
+  <si>
+    <t>A016_divipola</t>
+  </si>
+  <si>
+    <t>A016_estadoRegistro</t>
+  </si>
+  <si>
+    <t>id del registro</t>
+  </si>
+  <si>
+    <t>nombre departamental</t>
+  </si>
+  <si>
+    <t>DIVIPOLA asignado</t>
+  </si>
+  <si>
+    <t>Estado A:Activo</t>
+  </si>
+  <si>
+    <t>Listar muncipios disponibles para incluir en el departamental</t>
+  </si>
+  <si>
+    <t>departamental</t>
+  </si>
+  <si>
+    <t>A013_codigo</t>
+  </si>
+  <si>
+    <t>id municipio</t>
+  </si>
+  <si>
+    <t>nombre del municipio</t>
+  </si>
+  <si>
+    <t>parametro/listarMunDisponiblesDptal</t>
+  </si>
+  <si>
+    <t>parametro/listarMunicipiosDptal</t>
+  </si>
+  <si>
+    <t>Listar municipios que hacen parte de un departamental</t>
+  </si>
+  <si>
+    <t>id del departamental, 0 si es nuevo</t>
+  </si>
+  <si>
+    <t>id del departamental, o si es nuevo</t>
   </si>
 </sst>
 </file>
@@ -7353,6 +7471,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing39.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>370474</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>123071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="5143500"/>
+          <a:ext cx="8009524" cy="6028571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -8135,8 +8296,8 @@
       <xdr:rowOff>140806</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>405634</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>66047</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>91110</xdr:rowOff>
     </xdr:to>
@@ -8173,8 +8334,8 @@
       <xdr:rowOff>24848</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>654326</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>314739</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>49644</xdr:rowOff>
     </xdr:to>
@@ -15486,10 +15647,10 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja12"/>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15938,6 +16099,70 @@
       <c r="D28" t="str">
         <f>'HISTORIA 72'!C10</f>
         <v>Parametrizar entrega de carte a POLCA</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="36">
+        <v>18</v>
+      </c>
+      <c r="B29" t="str">
+        <f>'SERVICIO 18'!C6</f>
+        <v>deuda/editarDetalleEntregaCartera</v>
+      </c>
+      <c r="C29" s="36">
+        <v>72</v>
+      </c>
+      <c r="D29" t="str">
+        <f>'HISTORIA 72'!C10</f>
+        <v>Parametrizar entrega de carte a POLCA</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="36">
+        <v>19</v>
+      </c>
+      <c r="B30" t="str">
+        <f>'SERVICIO 19'!C6</f>
+        <v>parametro/listarDepartamentales</v>
+      </c>
+      <c r="C30" s="36">
+        <v>75</v>
+      </c>
+      <c r="D30" t="str">
+        <f>'HISTORIA 75'!C10</f>
+        <v>Paramerizar departamentales</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="36">
+        <v>20</v>
+      </c>
+      <c r="B31" t="str">
+        <f>'SERVICIO 20'!C6</f>
+        <v>parametro/listarMunDisponiblesDptal</v>
+      </c>
+      <c r="C31" s="36">
+        <v>75</v>
+      </c>
+      <c r="D31" t="str">
+        <f>'HISTORIA 75'!C10</f>
+        <v>Paramerizar departamentales</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="36">
+        <v>21</v>
+      </c>
+      <c r="B32" t="str">
+        <f>'SERVICIO 21'!C6</f>
+        <v>parametro/listarMunicipiosDptal</v>
+      </c>
+      <c r="C32" s="36">
+        <v>75</v>
+      </c>
+      <c r="D32" t="str">
+        <f>'HISTORIA 75'!C10</f>
+        <v>Paramerizar departamentales</v>
       </c>
     </row>
   </sheetData>
@@ -15999,6 +16224,14 @@
     <hyperlink ref="A27" location="'SERVICIO 16'!A1" display="'SERVICIO 16'!A1"/>
     <hyperlink ref="C28" location="'HISTORIA 72'!A1" display="'HISTORIA 72'!A1"/>
     <hyperlink ref="A28" location="'SERVICIO 17'!A1" display="'SERVICIO 17'!A1"/>
+    <hyperlink ref="C29" location="'HISTORIA 72'!A1" display="'HISTORIA 72'!A1"/>
+    <hyperlink ref="A29" location="'SERVICIO 18'!A1" display="'SERVICIO 18'!A1"/>
+    <hyperlink ref="A30" location="'SERVICIO 19'!A1" display="'SERVICIO 19'!A1"/>
+    <hyperlink ref="A31" location="'SERVICIO 20'!A1" display="'SERVICIO 20'!A1"/>
+    <hyperlink ref="A32" location="'SERVICIO 21'!A1" display="'SERVICIO 21'!A1"/>
+    <hyperlink ref="C30" location="'HISTORIA 75'!A1" display="'HISTORIA 75'!A1"/>
+    <hyperlink ref="C31" location="'HISTORIA 75'!A1" display="'HISTORIA 75'!A1"/>
+    <hyperlink ref="C32" location="'HISTORIA 75'!A1" display="'HISTORIA 75'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
@@ -24173,7 +24406,7 @@
   <dimension ref="A1:AF23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24664,6 +24897,7 @@
     <hyperlink ref="A16" location="'HISTORIA 77'!A1" display="'HISTORIA 77'!A1"/>
     <hyperlink ref="A17" location="'HISTORIA 78'!A1" display="'HISTORIA 78'!A1"/>
     <hyperlink ref="A18" location="'HISTORIA 79'!A1" display="'HISTORIA 79'!A1"/>
+    <hyperlink ref="A14" location="'HISTORIA 75'!A1" display="'HISTORIA 75'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
@@ -25282,8 +25516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G26"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27049,7 +27283,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -27411,6 +27647,287 @@
   <hyperlinks>
     <hyperlink ref="G4" location="SERVICIOS!A1" display="Lista Servicios"/>
     <hyperlink ref="C34" location="'HISTORIA 72'!A1" display="'HISTORIA 72'!A1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:G25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="106" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" s="107"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="108"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="25"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="37" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="C5" s="23">
+        <v>18</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="26"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>514</v>
+      </c>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="31"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="109" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="110"/>
+      <c r="D7" s="110"/>
+      <c r="E7" s="110"/>
+      <c r="F7" s="110"/>
+      <c r="G7" s="111"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="40" t="s">
+        <v>521</v>
+      </c>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="39"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="40"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="39"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="109" t="s">
+        <v>149</v>
+      </c>
+      <c r="C10" s="110"/>
+      <c r="D10" s="110"/>
+      <c r="E10" s="110"/>
+      <c r="F10" s="110"/>
+      <c r="G10" s="111"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="26"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="25" t="s">
+        <v>323</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>515</v>
+      </c>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="26"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="23" t="s">
+        <v>475</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>516</v>
+      </c>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="26"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="23" t="s">
+        <v>477</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>517</v>
+      </c>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="26"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="23" t="s">
+        <v>518</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>519</v>
+      </c>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="26"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="23" t="s">
+        <v>293</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>520</v>
+      </c>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="26"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="26"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="109" t="s">
+        <v>150</v>
+      </c>
+      <c r="C18" s="110"/>
+      <c r="D18" s="110"/>
+      <c r="E18" s="110"/>
+      <c r="F18" s="110"/>
+      <c r="G18" s="111"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="C19" s="23">
+        <v>0</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="26"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="25"/>
+      <c r="C20" s="42" t="s">
+        <v>179</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="26"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="26"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="25"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="26"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="25"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="26"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="109" t="s">
+        <v>167</v>
+      </c>
+      <c r="C24" s="110"/>
+      <c r="D24" s="110"/>
+      <c r="E24" s="110"/>
+      <c r="F24" s="110"/>
+      <c r="G24" s="111"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="32" t="s">
+        <v>168</v>
+      </c>
+      <c r="C25" s="36">
+        <v>72</v>
+      </c>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="34"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B24:G24"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G4" location="SERVICIOS!A1" display="Lista Servicios"/>
+    <hyperlink ref="C25" location="'HISTORIA 72'!A1" display="'HISTORIA 72'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
@@ -28233,6 +28750,902 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:G28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="106" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" s="107"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="108"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="25"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="37" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="C5" s="23">
+        <v>19</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="26"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>532</v>
+      </c>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="31"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="109" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="110"/>
+      <c r="D7" s="110"/>
+      <c r="E7" s="110"/>
+      <c r="F7" s="110"/>
+      <c r="G7" s="111"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="40" t="s">
+        <v>533</v>
+      </c>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="39"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="40"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="39"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="109" t="s">
+        <v>149</v>
+      </c>
+      <c r="C10" s="110"/>
+      <c r="D10" s="110"/>
+      <c r="E10" s="110"/>
+      <c r="F10" s="110"/>
+      <c r="G10" s="111"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="26"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="25"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="26"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="26"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="109" t="s">
+        <v>150</v>
+      </c>
+      <c r="C14" s="110"/>
+      <c r="D14" s="110"/>
+      <c r="E14" s="110"/>
+      <c r="F14" s="110"/>
+      <c r="G14" s="111"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="C15" s="23">
+        <v>0</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="26"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="25"/>
+      <c r="C16" s="42" t="s">
+        <v>179</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="26"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="26"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="25" t="s">
+        <v>472</v>
+      </c>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="26"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="25"/>
+      <c r="C19" s="23" t="s">
+        <v>534</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>538</v>
+      </c>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="26"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="25"/>
+      <c r="C20" s="23" t="s">
+        <v>535</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>539</v>
+      </c>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="26"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="25"/>
+      <c r="C21" s="23" t="s">
+        <v>536</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>540</v>
+      </c>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="26"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="25"/>
+      <c r="C22" s="23" t="s">
+        <v>537</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>541</v>
+      </c>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="26"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="25"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="26"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="25"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="26"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="25"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="26"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="25"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="26"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="109" t="s">
+        <v>167</v>
+      </c>
+      <c r="C27" s="110"/>
+      <c r="D27" s="110"/>
+      <c r="E27" s="110"/>
+      <c r="F27" s="110"/>
+      <c r="G27" s="111"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="32" t="s">
+        <v>168</v>
+      </c>
+      <c r="C28" s="36">
+        <v>75</v>
+      </c>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="34"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B27:G27"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G4" location="SERVICIOS!A1" display="Lista Servicios"/>
+    <hyperlink ref="C28" location="'HISTORIA 75'!A1" display="'HISTORIA 75'!A1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:G28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="106" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" s="107"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="108"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="25"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="37" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="C5" s="23">
+        <v>20</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="26"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>547</v>
+      </c>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="31"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="109" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="110"/>
+      <c r="D7" s="110"/>
+      <c r="E7" s="110"/>
+      <c r="F7" s="110"/>
+      <c r="G7" s="111"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="40" t="s">
+        <v>542</v>
+      </c>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="39"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="40"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="39"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="109" t="s">
+        <v>149</v>
+      </c>
+      <c r="C10" s="110"/>
+      <c r="D10" s="110"/>
+      <c r="E10" s="110"/>
+      <c r="F10" s="110"/>
+      <c r="G10" s="111"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="26"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="25" t="s">
+        <v>543</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>551</v>
+      </c>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="26"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="26"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="109" t="s">
+        <v>150</v>
+      </c>
+      <c r="C14" s="110"/>
+      <c r="D14" s="110"/>
+      <c r="E14" s="110"/>
+      <c r="F14" s="110"/>
+      <c r="G14" s="111"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="C15" s="23">
+        <v>0</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="26"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="25"/>
+      <c r="C16" s="42" t="s">
+        <v>179</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="26"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="26"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="25" t="s">
+        <v>472</v>
+      </c>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="26"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="25"/>
+      <c r="C19" s="23" t="s">
+        <v>544</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>545</v>
+      </c>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="26"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="25"/>
+      <c r="C20" s="23" t="s">
+        <v>505</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>546</v>
+      </c>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="26"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="25"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="26"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="25"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="26"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="25"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="26"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="25"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="26"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="25"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="26"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="25"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="26"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="109" t="s">
+        <v>167</v>
+      </c>
+      <c r="C27" s="110"/>
+      <c r="D27" s="110"/>
+      <c r="E27" s="110"/>
+      <c r="F27" s="110"/>
+      <c r="G27" s="111"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="32" t="s">
+        <v>168</v>
+      </c>
+      <c r="C28" s="36">
+        <v>75</v>
+      </c>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="34"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B27:G27"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G4" location="SERVICIOS!A1" display="Lista Servicios"/>
+    <hyperlink ref="C28" location="'HISTORIA 75'!A1" display="'HISTORIA 75'!A1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:G28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="106" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" s="107"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="108"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="25"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="37" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="C5" s="23">
+        <v>21</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="26"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>548</v>
+      </c>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="31"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="109" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="110"/>
+      <c r="D7" s="110"/>
+      <c r="E7" s="110"/>
+      <c r="F7" s="110"/>
+      <c r="G7" s="111"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="40" t="s">
+        <v>549</v>
+      </c>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="39"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="40"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="39"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="109" t="s">
+        <v>149</v>
+      </c>
+      <c r="C10" s="110"/>
+      <c r="D10" s="110"/>
+      <c r="E10" s="110"/>
+      <c r="F10" s="110"/>
+      <c r="G10" s="111"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="26"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="25" t="s">
+        <v>543</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>550</v>
+      </c>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="26"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="26"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="109" t="s">
+        <v>150</v>
+      </c>
+      <c r="C14" s="110"/>
+      <c r="D14" s="110"/>
+      <c r="E14" s="110"/>
+      <c r="F14" s="110"/>
+      <c r="G14" s="111"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="C15" s="23">
+        <v>0</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="26"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="25"/>
+      <c r="C16" s="42" t="s">
+        <v>179</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="26"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="26"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="25" t="s">
+        <v>472</v>
+      </c>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="26"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="25"/>
+      <c r="C19" s="23" t="s">
+        <v>544</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>545</v>
+      </c>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="26"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="25"/>
+      <c r="C20" s="23" t="s">
+        <v>505</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>546</v>
+      </c>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="26"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="25"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="26"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="25"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="26"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="25"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="26"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="25"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="26"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="25"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="26"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="25"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="26"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="109" t="s">
+        <v>167</v>
+      </c>
+      <c r="C27" s="110"/>
+      <c r="D27" s="110"/>
+      <c r="E27" s="110"/>
+      <c r="F27" s="110"/>
+      <c r="G27" s="111"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="32" t="s">
+        <v>168</v>
+      </c>
+      <c r="C28" s="36">
+        <v>75</v>
+      </c>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="34"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B27:G27"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G4" location="SERVICIOS!A1" display="Lista Servicios"/>
+    <hyperlink ref="C28" location="'HISTORIA 75'!A1" display="'HISTORIA 75'!A1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -29069,9 +30482,7 @@
   <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:R112"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -29787,7 +31198,15 @@
         <v>deuda/listarDetalleEntregaCartera</v>
       </c>
     </row>
-    <row r="110" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B110" s="12">
+        <v>18</v>
+      </c>
+      <c r="C110" s="7" t="str">
+        <f>'SERVICIO 18'!C6</f>
+        <v>deuda/editarDetalleEntregaCartera</v>
+      </c>
+    </row>
     <row r="111" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="112" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -29836,6 +31255,7 @@
     <hyperlink ref="B107" location="'SERVICIO 15'!A1" display="'SERVICIO 15'!A1"/>
     <hyperlink ref="B108" location="'SERVICIO 16'!A1" display="'SERVICIO 16'!A1"/>
     <hyperlink ref="B109" location="'SERVICIO 17'!A1" display="'SERVICIO 17'!A1"/>
+    <hyperlink ref="B110" location="'SERVICIO 18'!A1" display="'SERVICIO 18'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
@@ -30637,9 +32057,7 @@
   <sheetPr codeName="Hoja8"/>
   <dimension ref="A1:R108"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -31425,15 +32843,16 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja9"/>
-  <dimension ref="A1:R108"/>
+  <dimension ref="A1:R114"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
     <col min="5" max="5" width="26.140625" customWidth="1"/>
     <col min="9" max="18" width="11.42578125" style="7"/>
   </cols>
@@ -32182,32 +33601,125 @@
       <c r="F70" s="102"/>
       <c r="G70" s="103"/>
     </row>
-    <row r="71" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="78" t="s">
+        <v>460</v>
+      </c>
+      <c r="C71" s="78"/>
+      <c r="D71" s="78"/>
+      <c r="E71" s="78"/>
+      <c r="F71" s="78"/>
+      <c r="G71" s="78"/>
+    </row>
+    <row r="72" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="12">
+        <v>19</v>
+      </c>
+      <c r="C72" s="7" t="str">
+        <f>'SERVICIO 19'!C6</f>
+        <v>parametro/listarDepartamentales</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="12">
+        <v>20</v>
+      </c>
+      <c r="C73" s="7" t="str">
+        <f>'SERVICIO 20'!C6</f>
+        <v>parametro/listarMunDisponiblesDptal</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="12">
+        <v>21</v>
+      </c>
+      <c r="C74" s="7" t="str">
+        <f>'SERVICIO 21'!C6</f>
+        <v>parametro/listarMunicipiosDptal</v>
+      </c>
+    </row>
     <row r="75" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="76" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="77" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="88" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="90" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="91" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="7" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="7" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="7" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="7" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="36">
+        <v>5</v>
+      </c>
+      <c r="C83" t="s">
+        <v>318</v>
+      </c>
+      <c r="D83" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="7" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="7" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="2:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="7" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="7" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="7" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="7" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="2:4" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="2:4" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" spans="2:4" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="2:4" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="2:4" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="97" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="98" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="99" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -32220,8 +33732,15 @@
     <row r="106" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="107" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="108" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="110" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="111" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="112" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="113" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="26">
+    <mergeCell ref="B71:G71"/>
     <mergeCell ref="B18:G18"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="B7:G7"/>
@@ -32261,6 +33780,10 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="G5" location="'TAREAS ITERACION 2'!A1" display="Regresar Lista"/>
+    <hyperlink ref="B83" location="'SERVICIO 5'!A1" display="'SERVICIO 5'!A1"/>
+    <hyperlink ref="B72" location="'SERVICIO 19'!A1" display="'SERVICIO 19'!A1"/>
+    <hyperlink ref="B73" location="'SERVICIO 20'!A1" display="'SERVICIO 20'!A1"/>
+    <hyperlink ref="B74" location="'SERVICIO 21'!A1" display="'SERVICIO 21'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>

</xml_diff>